<commit_message>
clean for package; prepare backtest in sample changes
</commit_message>
<xml_diff>
--- a/Examples/summary_ic1000000_tc0.003_rf0.xlsx
+++ b/Examples/summary_ic1000000_tc0.003_rf0.xlsx
@@ -474,22 +474,22 @@
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>0.1035075999999999</v>
+        <v>0.1035075999999995</v>
       </c>
       <c r="D2" s="1">
-        <v>0.071998924304715</v>
+        <v>0.07199892430471455</v>
       </c>
       <c r="E2">
-        <v>1.162558000072732</v>
+        <v>1.16255800007273</v>
       </c>
       <c r="F2">
-        <v>0.9781149579882168</v>
+        <v>0.9781149579882155</v>
       </c>
       <c r="G2" s="1">
-        <v>0.07408878148230415</v>
+        <v>0.07408878148230398</v>
       </c>
       <c r="H2" s="1">
-        <v>0.04475908423671826</v>
+        <v>0.04475908423671837</v>
       </c>
       <c r="I2" t="s">
         <v>10</v>
@@ -544,13 +544,13 @@
         <v>37805</v>
       </c>
       <c r="B3">
-        <v>993818.5000000001</v>
+        <v>993818.5</v>
       </c>
       <c r="C3" s="1">
-        <v>-0.00618149999999984</v>
+        <v>-0.006181499999999951</v>
       </c>
       <c r="D3" s="1">
-        <v>-0.00618149999999984</v>
+        <v>-0.006181499999999951</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -558,13 +558,13 @@
         <v>37806</v>
       </c>
       <c r="B4">
-        <v>993818.5000000001</v>
+        <v>993818.5</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>-0.00618149999999984</v>
+        <v>-0.006181499999999951</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -572,13 +572,13 @@
         <v>37807</v>
       </c>
       <c r="B5">
-        <v>993818.5000000001</v>
+        <v>993818.5</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>-0.00618149999999984</v>
+        <v>-0.006181499999999951</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -586,13 +586,13 @@
         <v>37808</v>
       </c>
       <c r="B6">
-        <v>993818.5000000001</v>
+        <v>993818.5</v>
       </c>
       <c r="C6" s="1">
         <v>0</v>
       </c>
       <c r="D6" s="1">
-        <v>-0.00618149999999984</v>
+        <v>-0.006181499999999951</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -603,10 +603,10 @@
         <v>1003595.6</v>
       </c>
       <c r="C7" s="1">
-        <v>0.009837913059577819</v>
+        <v>0.009837913059577597</v>
       </c>
       <c r="D7" s="1">
-        <v>0.003595600000000143</v>
+        <v>0.003595599999999921</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -617,10 +617,10 @@
         <v>1003208.81</v>
       </c>
       <c r="C8" s="1">
-        <v>-0.0003854042405125879</v>
+        <v>-0.0003854042405126989</v>
       </c>
       <c r="D8" s="1">
-        <v>0.003208810000000284</v>
+        <v>0.003208810000000062</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -628,13 +628,13 @@
         <v>37811</v>
       </c>
       <c r="B9">
-        <v>997237.1300000005</v>
+        <v>997237.13</v>
       </c>
       <c r="C9" s="1">
-        <v>-0.005952579304003391</v>
+        <v>-0.005952579304003502</v>
       </c>
       <c r="D9" s="1">
-        <v>-0.00276286999999964</v>
+        <v>-0.002762869999999973</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -642,13 +642,13 @@
         <v>37812</v>
       </c>
       <c r="B10">
-        <v>987842.7800000004</v>
+        <v>987842.78</v>
       </c>
       <c r="C10" s="1">
-        <v>-0.009420377277769565</v>
+        <v>-0.009420377277769454</v>
       </c>
       <c r="D10" s="1">
-        <v>-0.01215721999999975</v>
+        <v>-0.01215721999999997</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -656,13 +656,13 @@
         <v>37813</v>
       </c>
       <c r="B11">
-        <v>994808.7700000005</v>
+        <v>994808.7700000001</v>
       </c>
       <c r="C11" s="1">
         <v>0.007051719302944237</v>
       </c>
       <c r="D11" s="1">
-        <v>-0.005191229999999658</v>
+        <v>-0.00519122999999988</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -670,13 +670,13 @@
         <v>37814</v>
       </c>
       <c r="B12">
-        <v>994808.7700000005</v>
+        <v>994808.7700000001</v>
       </c>
       <c r="C12" s="1">
         <v>0</v>
       </c>
       <c r="D12" s="1">
-        <v>-0.005191229999999658</v>
+        <v>-0.00519122999999988</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -684,13 +684,13 @@
         <v>37815</v>
       </c>
       <c r="B13">
-        <v>994808.7700000005</v>
+        <v>994808.7700000001</v>
       </c>
       <c r="C13" s="1">
         <v>0</v>
       </c>
       <c r="D13" s="1">
-        <v>-0.005191229999999658</v>
+        <v>-0.00519122999999988</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -698,13 +698,13 @@
         <v>37816</v>
       </c>
       <c r="B14">
-        <v>996540.1600000004</v>
+        <v>996540.1600000001</v>
       </c>
       <c r="C14" s="1">
         <v>0.00174042494619342</v>
       </c>
       <c r="D14" s="1">
-        <v>-0.003459839999999659</v>
+        <v>-0.003459839999999881</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -712,13 +712,13 @@
         <v>37817</v>
       </c>
       <c r="B15">
-        <v>992765.9200000004</v>
+        <v>992765.92</v>
       </c>
       <c r="C15" s="1">
-        <v>-0.003787343602891013</v>
+        <v>-0.003787343602891124</v>
       </c>
       <c r="D15" s="1">
-        <v>-0.007234079999999699</v>
+        <v>-0.007234080000000032</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -726,13 +726,13 @@
         <v>37818</v>
       </c>
       <c r="B16">
-        <v>985004.8800000002</v>
+        <v>985004.8799999999</v>
       </c>
       <c r="C16" s="1">
         <v>-0.007817593093848552</v>
       </c>
       <c r="D16" s="1">
-        <v>-0.01499511999999992</v>
+        <v>-0.01499512000000025</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -740,13 +740,13 @@
         <v>37819</v>
       </c>
       <c r="B17">
-        <v>979315.4800000002</v>
+        <v>979315.4799999999</v>
       </c>
       <c r="C17" s="1">
         <v>-0.005776011992955854</v>
       </c>
       <c r="D17" s="1">
-        <v>-0.02068451999999998</v>
+        <v>-0.02068452000000032</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -754,13 +754,13 @@
         <v>37820</v>
       </c>
       <c r="B18">
-        <v>988474.2900000004</v>
+        <v>988474.29</v>
       </c>
       <c r="C18" s="1">
         <v>0.009352256945841519</v>
       </c>
       <c r="D18" s="1">
-        <v>-0.01152570999999991</v>
+        <v>-0.01152571000000024</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -768,13 +768,13 @@
         <v>37821</v>
       </c>
       <c r="B19">
-        <v>988474.2900000004</v>
+        <v>988474.29</v>
       </c>
       <c r="C19" s="1">
         <v>0</v>
       </c>
       <c r="D19" s="1">
-        <v>-0.01152570999999991</v>
+        <v>-0.01152571000000024</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -782,13 +782,13 @@
         <v>37822</v>
       </c>
       <c r="B20">
-        <v>988474.2900000004</v>
+        <v>988474.29</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
       </c>
       <c r="D20" s="1">
-        <v>-0.01152570999999991</v>
+        <v>-0.01152571000000024</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -796,13 +796,13 @@
         <v>37823</v>
       </c>
       <c r="B21">
-        <v>975656.8300000004</v>
+        <v>975656.8300000001</v>
       </c>
       <c r="C21" s="1">
         <v>-0.01296691287742036</v>
       </c>
       <c r="D21" s="1">
-        <v>-0.02434316999999986</v>
+        <v>-0.02434317000000019</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -810,13 +810,13 @@
         <v>37824</v>
       </c>
       <c r="B22">
-        <v>981604.2200000003</v>
+        <v>981604.2199999999</v>
       </c>
       <c r="C22" s="1">
-        <v>0.006095780624012948</v>
+        <v>0.006095780624012725</v>
       </c>
       <c r="D22" s="1">
-        <v>-0.01839577999999997</v>
+        <v>-0.01839578000000053</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -824,13 +824,13 @@
         <v>37825</v>
       </c>
       <c r="B23">
-        <v>982734.7100000004</v>
+        <v>982734.7099999998</v>
       </c>
       <c r="C23" s="1">
-        <v>0.001151675977921318</v>
+        <v>0.001151675977921096</v>
       </c>
       <c r="D23" s="1">
-        <v>-0.01726528999999977</v>
+        <v>-0.01726529000000054</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -838,13 +838,13 @@
         <v>37826</v>
       </c>
       <c r="B24">
-        <v>977164.2100000004</v>
+        <v>977164.21</v>
       </c>
       <c r="C24" s="1">
-        <v>-0.00566836598251419</v>
+        <v>-0.005668365982514079</v>
       </c>
       <c r="D24" s="1">
-        <v>-0.02283578999999969</v>
+        <v>-0.02283579000000036</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -852,13 +852,13 @@
         <v>37827</v>
       </c>
       <c r="B25">
-        <v>986798.2100000004</v>
+        <v>986798.2099999997</v>
       </c>
       <c r="C25" s="1">
-        <v>0.009859141279846995</v>
+        <v>0.009859141279846773</v>
       </c>
       <c r="D25" s="1">
-        <v>-0.01320178999999966</v>
+        <v>-0.01320179000000055</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -866,13 +866,13 @@
         <v>37828</v>
       </c>
       <c r="B26">
-        <v>986798.2100000004</v>
+        <v>986798.2099999997</v>
       </c>
       <c r="C26" s="1">
         <v>0</v>
       </c>
       <c r="D26" s="1">
-        <v>-0.01320178999999966</v>
+        <v>-0.01320179000000055</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -880,13 +880,13 @@
         <v>37829</v>
       </c>
       <c r="B27">
-        <v>986798.2100000004</v>
+        <v>986798.2099999997</v>
       </c>
       <c r="C27" s="1">
         <v>0</v>
       </c>
       <c r="D27" s="1">
-        <v>-0.01320178999999966</v>
+        <v>-0.01320179000000055</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -894,13 +894,13 @@
         <v>37830</v>
       </c>
       <c r="B28">
-        <v>983721.4000000005</v>
+        <v>983721.3999999998</v>
       </c>
       <c r="C28" s="1">
         <v>-0.003117972822427317</v>
       </c>
       <c r="D28" s="1">
-        <v>-0.01627859999999959</v>
+        <v>-0.01627860000000048</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -908,13 +908,13 @@
         <v>37831</v>
       </c>
       <c r="B29">
-        <v>979015.9200000005</v>
+        <v>979015.9199999998</v>
       </c>
       <c r="C29" s="1">
         <v>-0.004783346179111247</v>
       </c>
       <c r="D29" s="1">
-        <v>-0.02098407999999952</v>
+        <v>-0.0209840800000004</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -922,13 +922,13 @@
         <v>37832</v>
       </c>
       <c r="B30">
-        <v>980345.5000000005</v>
+        <v>980345.4999999999</v>
       </c>
       <c r="C30" s="1">
-        <v>0.001358078017771103</v>
+        <v>0.001358078017771325</v>
       </c>
       <c r="D30" s="1">
-        <v>-0.01965449999999958</v>
+        <v>-0.01965450000000024</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -936,13 +936,13 @@
         <v>37833</v>
       </c>
       <c r="B31">
-        <v>979199.3700000003</v>
+        <v>979199.37</v>
       </c>
       <c r="C31" s="1">
-        <v>-0.001169108237861205</v>
+        <v>-0.001169108237860872</v>
       </c>
       <c r="D31" s="1">
-        <v>-0.02080062999999976</v>
+        <v>-0.0208006300000001</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -950,13 +950,13 @@
         <v>37834</v>
       </c>
       <c r="B32">
-        <v>970209.0000000003</v>
+        <v>970208.9999999999</v>
       </c>
       <c r="C32" s="1">
-        <v>-0.009181347818881913</v>
+        <v>-0.009181347818882024</v>
       </c>
       <c r="D32" s="1">
-        <v>-0.02979099999999979</v>
+        <v>-0.02979100000000023</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -964,13 +964,13 @@
         <v>37835</v>
       </c>
       <c r="B33">
-        <v>970209.0000000003</v>
+        <v>970208.9999999999</v>
       </c>
       <c r="C33" s="1">
         <v>0</v>
       </c>
       <c r="D33" s="1">
-        <v>-0.02979099999999979</v>
+        <v>-0.02979100000000023</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -978,13 +978,13 @@
         <v>37836</v>
       </c>
       <c r="B34">
-        <v>970209.0000000003</v>
+        <v>970208.9999999999</v>
       </c>
       <c r="C34" s="1">
         <v>0</v>
       </c>
       <c r="D34" s="1">
-        <v>-0.02979099999999979</v>
+        <v>-0.02979100000000023</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -992,13 +992,13 @@
         <v>37837</v>
       </c>
       <c r="B35">
-        <v>973033.9100000003</v>
+        <v>973033.9099999999</v>
       </c>
       <c r="C35" s="1">
-        <v>0.00291165099478552</v>
+        <v>0.002911650994785742</v>
       </c>
       <c r="D35" s="1">
-        <v>-0.02696608999999994</v>
+        <v>-0.02696609000000016</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1006,13 +1006,13 @@
         <v>37838</v>
       </c>
       <c r="B36">
-        <v>958675.5800000003</v>
+        <v>958675.58</v>
       </c>
       <c r="C36" s="1">
         <v>-0.01475624832026656</v>
       </c>
       <c r="D36" s="1">
-        <v>-0.04132441999999981</v>
+        <v>-0.04132442000000003</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1020,13 +1020,13 @@
         <v>37839</v>
       </c>
       <c r="B37">
-        <v>960117.7500000002</v>
+        <v>960117.7499999999</v>
       </c>
       <c r="C37" s="1">
         <v>0.001504335804610735</v>
       </c>
       <c r="D37" s="1">
-        <v>-0.0398822499999999</v>
+        <v>-0.03988225000000012</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1034,13 +1034,13 @@
         <v>37840</v>
       </c>
       <c r="B38">
-        <v>970001.6000000002</v>
+        <v>970001.5999999997</v>
       </c>
       <c r="C38" s="1">
-        <v>0.01029441440906598</v>
+        <v>0.01029441440906576</v>
       </c>
       <c r="D38" s="1">
-        <v>-0.02999839999999987</v>
+        <v>-0.02999840000000031</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1048,13 +1048,13 @@
         <v>37841</v>
       </c>
       <c r="B39">
-        <v>972415.6800000003</v>
+        <v>972415.6799999998</v>
       </c>
       <c r="C39" s="1">
         <v>0.002488738162906179</v>
       </c>
       <c r="D39" s="1">
-        <v>-0.02758431999999977</v>
+        <v>-0.02758432000000022</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1062,13 +1062,13 @@
         <v>37842</v>
       </c>
       <c r="B40">
-        <v>972415.6800000003</v>
+        <v>972415.6799999998</v>
       </c>
       <c r="C40" s="1">
         <v>0</v>
       </c>
       <c r="D40" s="1">
-        <v>-0.02758431999999977</v>
+        <v>-0.02758432000000022</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1076,13 +1076,13 @@
         <v>37843</v>
       </c>
       <c r="B41">
-        <v>972415.6800000003</v>
+        <v>972415.6799999998</v>
       </c>
       <c r="C41" s="1">
         <v>0</v>
       </c>
       <c r="D41" s="1">
-        <v>-0.02758431999999977</v>
+        <v>-0.02758432000000022</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1090,13 +1090,13 @@
         <v>37844</v>
       </c>
       <c r="B42">
-        <v>974091.9400000001</v>
+        <v>974091.9399999997</v>
       </c>
       <c r="C42" s="1">
         <v>0.001723810130251913</v>
       </c>
       <c r="D42" s="1">
-        <v>-0.02590806000000001</v>
+        <v>-0.02590806000000045</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1104,13 +1104,13 @@
         <v>37845</v>
       </c>
       <c r="B43">
-        <v>980176.0700000002</v>
+        <v>980176.0699999997</v>
       </c>
       <c r="C43" s="1">
-        <v>0.006245950459255578</v>
+        <v>0.006245950459255356</v>
       </c>
       <c r="D43" s="1">
-        <v>-0.01982392999999982</v>
+        <v>-0.01982393000000049</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1118,13 +1118,13 @@
         <v>37846</v>
       </c>
       <c r="B44">
-        <v>972617.6900000002</v>
+        <v>972617.6899999997</v>
       </c>
       <c r="C44" s="1">
         <v>-0.00771124722520522</v>
       </c>
       <c r="D44" s="1">
-        <v>-0.02738230999999991</v>
+        <v>-0.02738231000000058</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1132,13 +1132,13 @@
         <v>37847</v>
       </c>
       <c r="B45">
-        <v>974612.6100000002</v>
+        <v>974612.6099999999</v>
       </c>
       <c r="C45" s="1">
         <v>0.002051083401536813</v>
       </c>
       <c r="D45" s="1">
-        <v>-0.02538738999999979</v>
+        <v>-0.02538739000000045</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1146,13 +1146,13 @@
         <v>37848</v>
       </c>
       <c r="B46">
-        <v>975916.7400000002</v>
+        <v>975916.7399999999</v>
       </c>
       <c r="C46" s="1">
         <v>0.001338100889131777</v>
       </c>
       <c r="D46" s="1">
-        <v>-0.02408325999999972</v>
+        <v>-0.02408326000000038</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1160,13 +1160,13 @@
         <v>37849</v>
       </c>
       <c r="B47">
-        <v>975916.7400000002</v>
+        <v>975916.7399999999</v>
       </c>
       <c r="C47" s="1">
         <v>0</v>
       </c>
       <c r="D47" s="1">
-        <v>-0.02408325999999972</v>
+        <v>-0.02408326000000038</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1174,13 +1174,13 @@
         <v>37850</v>
       </c>
       <c r="B48">
-        <v>975916.7400000002</v>
+        <v>975916.7399999999</v>
       </c>
       <c r="C48" s="1">
         <v>0</v>
       </c>
       <c r="D48" s="1">
-        <v>-0.02408325999999972</v>
+        <v>-0.02408326000000038</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1188,13 +1188,13 @@
         <v>37851</v>
       </c>
       <c r="B49">
-        <v>978558.6000000002</v>
+        <v>978558.6</v>
       </c>
       <c r="C49" s="1">
-        <v>0.002707054702227873</v>
+        <v>0.002707054702228096</v>
       </c>
       <c r="D49" s="1">
-        <v>-0.02144139999999983</v>
+        <v>-0.02144140000000028</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1205,10 +1205,10 @@
         <v>977380.0000000001</v>
       </c>
       <c r="C50" s="1">
-        <v>-0.00120442454851466</v>
+        <v>-0.001204424548514327</v>
       </c>
       <c r="D50" s="1">
-        <v>-0.02261999999999997</v>
+        <v>-0.02262000000000008</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1216,13 +1216,13 @@
         <v>37853</v>
       </c>
       <c r="B51">
-        <v>977397.2600000001</v>
+        <v>977397.2600000002</v>
       </c>
       <c r="C51" s="1">
         <v>1.765945691545312E-05</v>
       </c>
       <c r="D51" s="1">
-        <v>-0.02260273999999995</v>
+        <v>-0.02260274000000007</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1230,13 +1230,13 @@
         <v>37854</v>
       </c>
       <c r="B52">
-        <v>977263.4200000002</v>
+        <v>977263.4200000003</v>
       </c>
       <c r="C52" s="1">
         <v>-0.0001369351086578652</v>
       </c>
       <c r="D52" s="1">
-        <v>-0.02273658000000001</v>
+        <v>-0.02273658000000012</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1244,13 +1244,13 @@
         <v>37855</v>
       </c>
       <c r="B53">
-        <v>967344.6399999999</v>
+        <v>967344.64</v>
       </c>
       <c r="C53" s="1">
         <v>-0.01014954596376916</v>
       </c>
       <c r="D53" s="1">
-        <v>-0.03265536000000024</v>
+        <v>-0.03265536000000036</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1258,13 +1258,13 @@
         <v>37856</v>
       </c>
       <c r="B54">
-        <v>967344.6399999999</v>
+        <v>967344.64</v>
       </c>
       <c r="C54" s="1">
         <v>0</v>
       </c>
       <c r="D54" s="1">
-        <v>-0.03265536000000024</v>
+        <v>-0.03265536000000036</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1272,13 +1272,13 @@
         <v>37857</v>
       </c>
       <c r="B55">
-        <v>967344.6399999999</v>
+        <v>967344.64</v>
       </c>
       <c r="C55" s="1">
         <v>0</v>
       </c>
       <c r="D55" s="1">
-        <v>-0.03265536000000024</v>
+        <v>-0.03265536000000036</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1286,13 +1286,13 @@
         <v>37858</v>
       </c>
       <c r="B56">
-        <v>970787.7099999998</v>
+        <v>970787.71</v>
       </c>
       <c r="C56" s="1">
         <v>0.003559300230370877</v>
       </c>
       <c r="D56" s="1">
-        <v>-0.02921229000000025</v>
+        <v>-0.02921229000000036</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1303,10 +1303,10 @@
         <v>973143.84</v>
       </c>
       <c r="C57" s="1">
-        <v>0.002427029077243015</v>
+        <v>0.002427029077242793</v>
       </c>
       <c r="D57" s="1">
-        <v>-0.02685616000000013</v>
+        <v>-0.02685616000000046</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1314,13 +1314,13 @@
         <v>37860</v>
       </c>
       <c r="B58">
-        <v>972826.0399999999</v>
+        <v>972826.04</v>
       </c>
       <c r="C58" s="1">
-        <v>-0.0003265704276564918</v>
+        <v>-0.0003265704276563808</v>
       </c>
       <c r="D58" s="1">
-        <v>-0.02717396000000016</v>
+        <v>-0.02717396000000039</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1334,7 +1334,7 @@
         <v>0.003171440600006958</v>
       </c>
       <c r="D59" s="1">
-        <v>-0.02408870000000018</v>
+        <v>-0.02408870000000041</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1342,10 +1342,10 @@
         <v>37862</v>
       </c>
       <c r="B60">
-        <v>979723.9099999998</v>
+        <v>979723.9099999999</v>
       </c>
       <c r="C60" s="1">
-        <v>0.003906717751910316</v>
+        <v>0.003906717751910538</v>
       </c>
       <c r="D60" s="1">
         <v>-0.0202760900000003</v>
@@ -1356,7 +1356,7 @@
         <v>37863</v>
       </c>
       <c r="B61">
-        <v>979723.9099999998</v>
+        <v>979723.9099999999</v>
       </c>
       <c r="C61" s="1">
         <v>0</v>
@@ -1370,7 +1370,7 @@
         <v>37864</v>
       </c>
       <c r="B62">
-        <v>979723.9099999998</v>
+        <v>979723.9099999999</v>
       </c>
       <c r="C62" s="1">
         <v>0</v>
@@ -1384,7 +1384,7 @@
         <v>37865</v>
       </c>
       <c r="B63">
-        <v>979723.9099999998</v>
+        <v>979723.9099999999</v>
       </c>
       <c r="C63" s="1">
         <v>0</v>
@@ -1398,13 +1398,13 @@
         <v>37866</v>
       </c>
       <c r="B64">
-        <v>992469.13</v>
+        <v>992469.1299999999</v>
       </c>
       <c r="C64" s="1">
-        <v>0.01300899148210055</v>
+        <v>0.01300899148210033</v>
       </c>
       <c r="D64" s="1">
-        <v>-0.007530870000000078</v>
+        <v>-0.0075308700000003</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1418,7 +1418,7 @@
         <v>0.001855110596739706</v>
       </c>
       <c r="D65" s="1">
-        <v>-0.005689730000000059</v>
+        <v>-0.005689730000000282</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1432,7 +1432,7 @@
         <v>0.001341030099186069</v>
       </c>
       <c r="D66" s="1">
-        <v>-0.004356330000000241</v>
+        <v>-0.004356330000000463</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1446,7 +1446,7 @@
         <v>-0.004591713017168098</v>
       </c>
       <c r="D67" s="1">
-        <v>-0.008928040000000248</v>
+        <v>-0.00892804000000047</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1460,7 +1460,7 @@
         <v>0</v>
       </c>
       <c r="D68" s="1">
-        <v>-0.008928040000000248</v>
+        <v>-0.00892804000000047</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1474,7 +1474,7 @@
         <v>0</v>
       </c>
       <c r="D69" s="1">
-        <v>-0.008928040000000248</v>
+        <v>-0.00892804000000047</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1488,7 +1488,7 @@
         <v>0.009863491647972733</v>
       </c>
       <c r="D70" s="1">
-        <v>0.0008473899999996704</v>
+        <v>0.0008473899999994483</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1502,7 +1502,7 @@
         <v>-0.00552274008527931</v>
       </c>
       <c r="D71" s="1">
-        <v>-0.004680030000000501</v>
+        <v>-0.004680030000000723</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1510,13 +1510,13 @@
         <v>37874</v>
       </c>
       <c r="B72">
-        <v>993163.8299999997</v>
+        <v>993163.8299999998</v>
       </c>
       <c r="C72" s="1">
-        <v>-0.002166278247185294</v>
+        <v>-0.002166278247185183</v>
       </c>
       <c r="D72" s="1">
-        <v>-0.006836170000000585</v>
+        <v>-0.006836170000000696</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1527,10 +1527,10 @@
         <v>996570.7099999997</v>
       </c>
       <c r="C73" s="1">
-        <v>0.003430330321232189</v>
+        <v>0.003430330321231967</v>
       </c>
       <c r="D73" s="1">
-        <v>-0.003429290000000473</v>
+        <v>-0.003429290000000806</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1544,7 +1544,7 @@
         <v>0.002244476962402375</v>
       </c>
       <c r="D74" s="1">
-        <v>-0.001192510000000535</v>
+        <v>-0.001192510000000868</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1558,7 +1558,7 @@
         <v>0</v>
       </c>
       <c r="D75" s="1">
-        <v>-0.001192510000000535</v>
+        <v>-0.001192510000000868</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1572,7 +1572,7 @@
         <v>0</v>
       </c>
       <c r="D76" s="1">
-        <v>-0.001192510000000535</v>
+        <v>-0.001192510000000868</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1586,7 +1586,7 @@
         <v>-0.002917869588663358</v>
       </c>
       <c r="D77" s="1">
-        <v>-0.004106900000000691</v>
+        <v>-0.004106900000001024</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1597,10 +1597,10 @@
         <v>1003678.3</v>
       </c>
       <c r="C78" s="1">
-        <v>0.007817304889450538</v>
+        <v>0.00781730488945076</v>
       </c>
       <c r="D78" s="1">
-        <v>0.003678299999999357</v>
+        <v>0.003678299999999135</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1611,10 +1611,10 @@
         <v>1001688.7</v>
       </c>
       <c r="C79" s="1">
-        <v>-0.001982308474737238</v>
+        <v>-0.001982308474737571</v>
       </c>
       <c r="D79" s="1">
-        <v>0.001688699999999432</v>
+        <v>0.001688699999998988</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1625,10 +1625,10 @@
         <v>1010641.41</v>
       </c>
       <c r="C80" s="1">
-        <v>0.008937617046094193</v>
+        <v>0.008937617046094415</v>
       </c>
       <c r="D80" s="1">
-        <v>0.01064140999999941</v>
+        <v>0.01064140999999919</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1642,7 +1642,7 @@
         <v>-0.003923528128537579</v>
       </c>
       <c r="D81" s="1">
-        <v>0.006676129999999558</v>
+        <v>0.006676129999999336</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1656,7 +1656,7 @@
         <v>0</v>
       </c>
       <c r="D82" s="1">
-        <v>0.006676129999999558</v>
+        <v>0.006676129999999336</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1670,7 +1670,7 @@
         <v>0</v>
       </c>
       <c r="D83" s="1">
-        <v>0.006676129999999558</v>
+        <v>0.006676129999999336</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1684,7 +1684,7 @@
         <v>-0.009638939188912676</v>
       </c>
       <c r="D84" s="1">
-        <v>-0.003027160000000362</v>
+        <v>-0.003027160000000584</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1698,7 +1698,7 @@
         <v>0.005064149992290545</v>
       </c>
       <c r="D85" s="1">
-        <v>0.002021659999999592</v>
+        <v>0.00202165999999937</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1712,7 +1712,7 @@
         <v>-0.01291181669665686</v>
       </c>
       <c r="D86" s="1">
-        <v>-0.01091626000000023</v>
+        <v>-0.01091626000000046</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1726,7 +1726,7 @@
         <v>-0.003784108310182055</v>
       </c>
       <c r="D87" s="1">
-        <v>-0.01465906000000017</v>
+        <v>-0.01465906000000039</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1734,10 +1734,10 @@
         <v>37890</v>
       </c>
       <c r="B88">
-        <v>982872.6499999997</v>
+        <v>982872.6499999999</v>
       </c>
       <c r="C88" s="1">
-        <v>-0.002505011108135058</v>
+        <v>-0.002505011108134836</v>
       </c>
       <c r="D88" s="1">
         <v>-0.01712735000000043</v>
@@ -1748,7 +1748,7 @@
         <v>37891</v>
       </c>
       <c r="B89">
-        <v>982872.6499999997</v>
+        <v>982872.6499999999</v>
       </c>
       <c r="C89" s="1">
         <v>0</v>
@@ -1762,7 +1762,7 @@
         <v>37892</v>
       </c>
       <c r="B90">
-        <v>982872.6499999997</v>
+        <v>982872.6499999999</v>
       </c>
       <c r="C90" s="1">
         <v>0</v>
@@ -1776,7 +1776,7 @@
         <v>37893</v>
       </c>
       <c r="B91">
-        <v>990018.1599999997</v>
+        <v>990018.1599999999</v>
       </c>
       <c r="C91" s="1">
         <v>0.007270026284686981</v>
@@ -1790,7 +1790,7 @@
         <v>37894</v>
       </c>
       <c r="B92">
-        <v>983947.7999999997</v>
+        <v>983947.7999999999</v>
       </c>
       <c r="C92" s="1">
         <v>-0.006131564293729741</v>
@@ -1804,13 +1804,13 @@
         <v>37895</v>
       </c>
       <c r="B93">
-        <v>999603.0999999995</v>
+        <v>999603.0999999999</v>
       </c>
       <c r="C93" s="1">
-        <v>0.01591070176690246</v>
+        <v>0.01591070176690268</v>
       </c>
       <c r="D93" s="1">
-        <v>-0.0003969000000006995</v>
+        <v>-0.0003969000000004774</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -1821,7 +1821,7 @@
         <v>1002630.44</v>
       </c>
       <c r="C94" s="1">
-        <v>0.003028542028331138</v>
+        <v>0.003028542028330916</v>
       </c>
       <c r="D94" s="1">
         <v>0.002630439999999457</v>
@@ -1905,10 +1905,10 @@
         <v>1004319.99</v>
       </c>
       <c r="C100" s="1">
-        <v>-0.004060087449776373</v>
+        <v>-0.004060087449776706</v>
       </c>
       <c r="D100" s="1">
-        <v>0.004319989999999718</v>
+        <v>0.004319989999999496</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -1922,7 +1922,7 @@
         <v>0.002459793715745784</v>
       </c>
       <c r="D101" s="1">
-        <v>0.00679040999999958</v>
+        <v>0.006790409999999358</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -1933,7 +1933,7 @@
         <v>1005185.41</v>
       </c>
       <c r="C102" s="1">
-        <v>-0.001594174898825296</v>
+        <v>-0.001594174898825185</v>
       </c>
       <c r="D102" s="1">
         <v>0.005185409999999502</v>
@@ -2003,10 +2003,10 @@
         <v>1008584</v>
       </c>
       <c r="C107" s="1">
-        <v>-0.004278235887917647</v>
+        <v>-0.004278235887917869</v>
       </c>
       <c r="D107" s="1">
-        <v>0.008583999999999481</v>
+        <v>0.008583999999999259</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -2020,7 +2020,7 @@
         <v>0.003050306171821227</v>
       </c>
       <c r="D108" s="1">
-        <v>0.01166048999999969</v>
+        <v>0.01166048999999947</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -2034,7 +2034,7 @@
         <v>-0.007032418553777897</v>
       </c>
       <c r="D109" s="1">
-        <v>0.004546069999999736</v>
+        <v>0.004546069999999514</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -2048,7 +2048,7 @@
         <v>0</v>
       </c>
       <c r="D110" s="1">
-        <v>0.004546069999999736</v>
+        <v>0.004546069999999514</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2062,7 +2062,7 @@
         <v>0</v>
       </c>
       <c r="D111" s="1">
-        <v>0.004546069999999736</v>
+        <v>0.004546069999999514</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2076,7 +2076,7 @@
         <v>0.003582175180875335</v>
       </c>
       <c r="D112" s="1">
-        <v>0.008144529999999595</v>
+        <v>0.008144529999999373</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2090,7 +2090,7 @@
         <v>0.00285859806232347</v>
       </c>
       <c r="D113" s="1">
-        <v>0.01102640999999971</v>
+        <v>0.01102640999999926</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2098,13 +2098,13 @@
         <v>37916</v>
       </c>
       <c r="B114">
-        <v>997525.7999999998</v>
+        <v>997525.7999999996</v>
       </c>
       <c r="C114" s="1">
-        <v>-0.01335337026458117</v>
+        <v>-0.01335337026458105</v>
       </c>
       <c r="D114" s="1">
-        <v>-0.002474200000000537</v>
+        <v>-0.00247420000000087</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2118,7 +2118,7 @@
         <v>0.004347115633500431</v>
       </c>
       <c r="D115" s="1">
-        <v>0.001862159999999502</v>
+        <v>0.001862159999999058</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2129,10 +2129,10 @@
         <v>1000533.34</v>
       </c>
       <c r="C116" s="1">
-        <v>-0.001326350123853404</v>
+        <v>-0.001326350123853293</v>
       </c>
       <c r="D116" s="1">
-        <v>0.0005333399999993826</v>
+        <v>0.0005333399999991606</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2146,7 +2146,7 @@
         <v>0</v>
       </c>
       <c r="D117" s="1">
-        <v>0.0005333399999993826</v>
+        <v>0.0005333399999991606</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2160,7 +2160,7 @@
         <v>0</v>
       </c>
       <c r="D118" s="1">
-        <v>0.0005333399999993826</v>
+        <v>0.0005333399999991606</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2171,7 +2171,7 @@
         <v>1000403.57</v>
       </c>
       <c r="C119" s="1">
-        <v>-0.0001297008253619003</v>
+        <v>-0.0001297008253616783</v>
       </c>
       <c r="D119" s="1">
         <v>0.0004035699999993536</v>
@@ -2199,7 +2199,7 @@
         <v>1009056.76</v>
       </c>
       <c r="C121" s="1">
-        <v>-0.0004167997759553232</v>
+        <v>-0.0004167997759554343</v>
       </c>
       <c r="D121" s="1">
         <v>0.009056759999999331</v>
@@ -2213,10 +2213,10 @@
         <v>1007420.79</v>
       </c>
       <c r="C122" s="1">
-        <v>-0.001621286398200361</v>
+        <v>-0.00162128639820025</v>
       </c>
       <c r="D122" s="1">
-        <v>0.007420789999999178</v>
+        <v>0.0074207899999994</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2227,10 +2227,10 @@
         <v>1011825.52</v>
       </c>
       <c r="C123" s="1">
-        <v>0.004372284197152521</v>
+        <v>0.004372284197152743</v>
       </c>
       <c r="D123" s="1">
-        <v>0.01182551999999903</v>
+        <v>0.01182551999999948</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -2244,7 +2244,7 @@
         <v>0</v>
       </c>
       <c r="D124" s="1">
-        <v>0.01182551999999903</v>
+        <v>0.01182551999999948</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2258,7 +2258,7 @@
         <v>0</v>
       </c>
       <c r="D125" s="1">
-        <v>0.01182551999999903</v>
+        <v>0.01182551999999948</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -2272,7 +2272,7 @@
         <v>0.003571307432530313</v>
       </c>
       <c r="D126" s="1">
-        <v>0.01543905999999895</v>
+        <v>0.01543905999999939</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -2280,13 +2280,13 @@
         <v>37929</v>
       </c>
       <c r="B127">
-        <v>1008863.539999999</v>
+        <v>1008863.54</v>
       </c>
       <c r="C127" s="1">
-        <v>-0.006475543692400554</v>
+        <v>-0.006475543692400332</v>
       </c>
       <c r="D127" s="1">
-        <v>0.008863539999998782</v>
+        <v>0.008863539999999448</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2300,7 +2300,7 @@
         <v>4.141293479609232E-05</v>
       </c>
       <c r="D128" s="1">
-        <v>0.008905319999998884</v>
+        <v>0.00890531999999955</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -2311,10 +2311,10 @@
         <v>1012385.31</v>
       </c>
       <c r="C129" s="1">
-        <v>0.003449273119106921</v>
+        <v>0.003449273119106699</v>
       </c>
       <c r="D129" s="1">
-        <v>0.01238530999999887</v>
+        <v>0.01238530999999932</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2322,13 +2322,13 @@
         <v>37932</v>
       </c>
       <c r="B130">
-        <v>1007529.959999999</v>
+        <v>1007529.96</v>
       </c>
       <c r="C130" s="1">
-        <v>-0.004795950664278292</v>
+        <v>-0.00479595066427807</v>
       </c>
       <c r="D130" s="1">
-        <v>0.007529959999998725</v>
+        <v>0.007529959999999392</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -2336,13 +2336,13 @@
         <v>37933</v>
       </c>
       <c r="B131">
-        <v>1007529.959999999</v>
+        <v>1007529.96</v>
       </c>
       <c r="C131" s="1">
         <v>0</v>
       </c>
       <c r="D131" s="1">
-        <v>0.007529959999998725</v>
+        <v>0.007529959999999392</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -2350,13 +2350,13 @@
         <v>37934</v>
       </c>
       <c r="B132">
-        <v>1007529.959999999</v>
+        <v>1007529.96</v>
       </c>
       <c r="C132" s="1">
         <v>0</v>
       </c>
       <c r="D132" s="1">
-        <v>0.007529959999998725</v>
+        <v>0.007529959999999392</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -2364,13 +2364,13 @@
         <v>37935</v>
       </c>
       <c r="B133">
-        <v>1003184.839999999</v>
+        <v>1003184.84</v>
       </c>
       <c r="C133" s="1">
-        <v>-0.00431264594851366</v>
+        <v>-0.004312645948513438</v>
       </c>
       <c r="D133" s="1">
-        <v>0.003184839999998523</v>
+        <v>0.003184839999999411</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -2378,13 +2378,13 @@
         <v>37936</v>
       </c>
       <c r="B134">
-        <v>1004223.269999999</v>
+        <v>1004223.27</v>
       </c>
       <c r="C134" s="1">
         <v>0.001035133266168664</v>
       </c>
       <c r="D134" s="1">
-        <v>0.004223269999998669</v>
+        <v>0.004223269999999557</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -2392,13 +2392,13 @@
         <v>37937</v>
       </c>
       <c r="B135">
-        <v>1013655.539999999</v>
+        <v>1013655.54</v>
       </c>
       <c r="C135" s="1">
         <v>0.009392602503624392</v>
       </c>
       <c r="D135" s="1">
-        <v>0.01365553999999847</v>
+        <v>0.01365553999999936</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -2406,13 +2406,13 @@
         <v>37938</v>
       </c>
       <c r="B136">
-        <v>1019560.879999999</v>
+        <v>1019560.88</v>
       </c>
       <c r="C136" s="1">
         <v>0.00582578574966397</v>
       </c>
       <c r="D136" s="1">
-        <v>0.01956087999999845</v>
+        <v>0.01956087999999934</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -2420,13 +2420,13 @@
         <v>37939</v>
       </c>
       <c r="B137">
-        <v>1019546.639999999</v>
+        <v>1019546.64</v>
       </c>
       <c r="C137" s="1">
         <v>-1.396679715681692E-05</v>
       </c>
       <c r="D137" s="1">
-        <v>0.01954663999999839</v>
+        <v>0.01954663999999928</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -2434,13 +2434,13 @@
         <v>37940</v>
       </c>
       <c r="B138">
-        <v>1019546.639999999</v>
+        <v>1019546.64</v>
       </c>
       <c r="C138" s="1">
         <v>0</v>
       </c>
       <c r="D138" s="1">
-        <v>0.01954663999999839</v>
+        <v>0.01954663999999928</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -2448,13 +2448,13 @@
         <v>37941</v>
       </c>
       <c r="B139">
-        <v>1019546.639999999</v>
+        <v>1019546.64</v>
       </c>
       <c r="C139" s="1">
         <v>0</v>
       </c>
       <c r="D139" s="1">
-        <v>0.01954663999999839</v>
+        <v>0.01954663999999928</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -2462,13 +2462,13 @@
         <v>37942</v>
       </c>
       <c r="B140">
-        <v>1014981.159999999</v>
+        <v>1014981.16</v>
       </c>
       <c r="C140" s="1">
         <v>-0.0044779511018741</v>
       </c>
       <c r="D140" s="1">
-        <v>0.01498115999999827</v>
+        <v>0.01498115999999916</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -2476,13 +2476,13 @@
         <v>37943</v>
       </c>
       <c r="B141">
-        <v>1008208.309999999</v>
+        <v>1008208.31</v>
       </c>
       <c r="C141" s="1">
         <v>-0.006672882479907383</v>
       </c>
       <c r="D141" s="1">
-        <v>0.008208309999998109</v>
+        <v>0.008208309999998997</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -2490,13 +2490,13 @@
         <v>37944</v>
       </c>
       <c r="B142">
-        <v>1015897.229999999</v>
+        <v>1015897.23</v>
       </c>
       <c r="C142" s="1">
         <v>0.007626320794757335</v>
       </c>
       <c r="D142" s="1">
-        <v>0.01589722999999821</v>
+        <v>0.0158972299999991</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -2504,13 +2504,13 @@
         <v>37945</v>
       </c>
       <c r="B143">
-        <v>1007908.499999999</v>
+        <v>1007908.5</v>
       </c>
       <c r="C143" s="1">
-        <v>-0.007863718655872209</v>
+        <v>-0.007863718655872098</v>
       </c>
       <c r="D143" s="1">
-        <v>0.00790849999999832</v>
+        <v>0.007908499999999208</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -2518,13 +2518,13 @@
         <v>37946</v>
       </c>
       <c r="B144">
-        <v>1005712.269999999</v>
+        <v>1005712.27</v>
       </c>
       <c r="C144" s="1">
-        <v>-0.002178997399069571</v>
+        <v>-0.002178997399069682</v>
       </c>
       <c r="D144" s="1">
-        <v>0.005712269999998298</v>
+        <v>0.005712269999998965</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -2532,13 +2532,13 @@
         <v>37947</v>
       </c>
       <c r="B145">
-        <v>1005712.269999999</v>
+        <v>1005712.27</v>
       </c>
       <c r="C145" s="1">
         <v>0</v>
       </c>
       <c r="D145" s="1">
-        <v>0.005712269999998298</v>
+        <v>0.005712269999998965</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -2546,13 +2546,13 @@
         <v>37948</v>
       </c>
       <c r="B146">
-        <v>1005712.269999999</v>
+        <v>1005712.27</v>
       </c>
       <c r="C146" s="1">
         <v>0</v>
       </c>
       <c r="D146" s="1">
-        <v>0.005712269999998298</v>
+        <v>0.005712269999998965</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -2560,13 +2560,13 @@
         <v>37949</v>
       </c>
       <c r="B147">
-        <v>1018976.709999999</v>
+        <v>1018976.71</v>
       </c>
       <c r="C147" s="1">
-        <v>0.01318910029804043</v>
+        <v>0.01318910029804066</v>
       </c>
       <c r="D147" s="1">
-        <v>0.01897670999999823</v>
+        <v>0.01897670999999912</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -2574,13 +2574,13 @@
         <v>37950</v>
       </c>
       <c r="B148">
-        <v>1019121.489999999</v>
+        <v>1019121.49</v>
       </c>
       <c r="C148" s="1">
-        <v>0.0001420837184789026</v>
+        <v>0.0001420837184786805</v>
       </c>
       <c r="D148" s="1">
-        <v>0.01912148999999852</v>
+        <v>0.01912148999999919</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -2588,13 +2588,13 @@
         <v>37951</v>
       </c>
       <c r="B149">
-        <v>1021622.709999999</v>
+        <v>1021622.71</v>
       </c>
       <c r="C149" s="1">
         <v>0.002454290312335461</v>
       </c>
       <c r="D149" s="1">
-        <v>0.02162270999999838</v>
+        <v>0.02162270999999905</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -2602,13 +2602,13 @@
         <v>37952</v>
       </c>
       <c r="B150">
-        <v>1021622.709999999</v>
+        <v>1021622.71</v>
       </c>
       <c r="C150" s="1">
         <v>0</v>
       </c>
       <c r="D150" s="1">
-        <v>0.02162270999999838</v>
+        <v>0.02162270999999905</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -2616,13 +2616,13 @@
         <v>37953</v>
       </c>
       <c r="B151">
-        <v>1020772.329999999</v>
+        <v>1020772.33</v>
       </c>
       <c r="C151" s="1">
-        <v>-0.0008323816529096639</v>
+        <v>-0.0008323816529097749</v>
       </c>
       <c r="D151" s="1">
-        <v>0.02077232999999845</v>
+        <v>0.02077232999999912</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -2630,13 +2630,13 @@
         <v>37954</v>
       </c>
       <c r="B152">
-        <v>1020772.329999999</v>
+        <v>1020772.33</v>
       </c>
       <c r="C152" s="1">
         <v>0</v>
       </c>
       <c r="D152" s="1">
-        <v>0.02077232999999845</v>
+        <v>0.02077232999999912</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -2644,13 +2644,13 @@
         <v>37955</v>
       </c>
       <c r="B153">
-        <v>1020772.329999999</v>
+        <v>1020772.33</v>
       </c>
       <c r="C153" s="1">
         <v>0</v>
       </c>
       <c r="D153" s="1">
-        <v>0.02077232999999845</v>
+        <v>0.02077232999999912</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -2658,13 +2658,13 @@
         <v>37956</v>
       </c>
       <c r="B154">
-        <v>1030579.849999999</v>
+        <v>1030579.85</v>
       </c>
       <c r="C154" s="1">
-        <v>0.009607940685461225</v>
+        <v>0.009607940685461003</v>
       </c>
       <c r="D154" s="1">
-        <v>0.03057984999999852</v>
+        <v>0.03057984999999896</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -2672,13 +2672,13 @@
         <v>37957</v>
       </c>
       <c r="B155">
-        <v>1028337.769999999</v>
+        <v>1028337.77</v>
       </c>
       <c r="C155" s="1">
         <v>-0.002175551947770082</v>
       </c>
       <c r="D155" s="1">
-        <v>0.02833776999999849</v>
+        <v>0.02833776999999893</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -2686,13 +2686,13 @@
         <v>37958</v>
       </c>
       <c r="B156">
-        <v>1028195.999999999</v>
+        <v>1028196</v>
       </c>
       <c r="C156" s="1">
-        <v>-0.0001378632625737009</v>
+        <v>-0.0001378632625738119</v>
       </c>
       <c r="D156" s="1">
-        <v>0.02819599999999856</v>
+        <v>0.02819599999999878</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -2700,13 +2700,13 @@
         <v>37959</v>
       </c>
       <c r="B157">
-        <v>1031122.259999999</v>
+        <v>1031122.26</v>
       </c>
       <c r="C157" s="1">
-        <v>0.002846013795035018</v>
+        <v>0.00284601379503524</v>
       </c>
       <c r="D157" s="1">
-        <v>0.03112225999999829</v>
+        <v>0.03112225999999874</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -2714,13 +2714,13 @@
         <v>37960</v>
       </c>
       <c r="B158">
-        <v>1027198.569999999</v>
+        <v>1027198.57</v>
       </c>
       <c r="C158" s="1">
         <v>-0.003805261657332304</v>
       </c>
       <c r="D158" s="1">
-        <v>0.02719856999999837</v>
+        <v>0.02719856999999881</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -2728,13 +2728,13 @@
         <v>37961</v>
       </c>
       <c r="B159">
-        <v>1027198.569999999</v>
+        <v>1027198.57</v>
       </c>
       <c r="C159" s="1">
         <v>0</v>
       </c>
       <c r="D159" s="1">
-        <v>0.02719856999999837</v>
+        <v>0.02719856999999881</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -2742,13 +2742,13 @@
         <v>37962</v>
       </c>
       <c r="B160">
-        <v>1027198.569999999</v>
+        <v>1027198.57</v>
       </c>
       <c r="C160" s="1">
         <v>0</v>
       </c>
       <c r="D160" s="1">
-        <v>0.02719856999999837</v>
+        <v>0.02719856999999881</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -2756,13 +2756,13 @@
         <v>37963</v>
       </c>
       <c r="B161">
-        <v>1033213.039999999</v>
+        <v>1033213.04</v>
       </c>
       <c r="C161" s="1">
         <v>0.005855216484579095</v>
       </c>
       <c r="D161" s="1">
-        <v>0.03321303999999836</v>
+        <v>0.03321303999999881</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -2770,13 +2770,13 @@
         <v>37964</v>
       </c>
       <c r="B162">
-        <v>1027431.209999999</v>
+        <v>1027431.21</v>
       </c>
       <c r="C162" s="1">
         <v>-0.005595970798045635</v>
       </c>
       <c r="D162" s="1">
-        <v>0.02743120999999848</v>
+        <v>0.02743120999999893</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -2787,10 +2787,10 @@
         <v>1025815.84</v>
       </c>
       <c r="C163" s="1">
-        <v>-0.001572241512889261</v>
+        <v>-0.001572241512889372</v>
       </c>
       <c r="D163" s="1">
-        <v>0.02581583999999837</v>
+        <v>0.02581583999999881</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -2798,13 +2798,13 @@
         <v>37966</v>
       </c>
       <c r="B164">
-        <v>1033794.829999999</v>
+        <v>1033794.83</v>
       </c>
       <c r="C164" s="1">
         <v>0.007778189504268118</v>
       </c>
       <c r="D164" s="1">
-        <v>0.03379482999999839</v>
+        <v>0.03379482999999883</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -2812,13 +2812,13 @@
         <v>37967</v>
       </c>
       <c r="B165">
-        <v>1035515.919999999</v>
+        <v>1035515.92</v>
       </c>
       <c r="C165" s="1">
         <v>0.001664827439696204</v>
       </c>
       <c r="D165" s="1">
-        <v>0.03551591999999837</v>
+        <v>0.03551591999999881</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -2826,13 +2826,13 @@
         <v>37968</v>
       </c>
       <c r="B166">
-        <v>1035515.919999999</v>
+        <v>1035515.92</v>
       </c>
       <c r="C166" s="1">
         <v>0</v>
       </c>
       <c r="D166" s="1">
-        <v>0.03551591999999837</v>
+        <v>0.03551591999999881</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -2840,13 +2840,13 @@
         <v>37969</v>
       </c>
       <c r="B167">
-        <v>1035515.919999999</v>
+        <v>1035515.92</v>
       </c>
       <c r="C167" s="1">
         <v>0</v>
       </c>
       <c r="D167" s="1">
-        <v>0.03551591999999837</v>
+        <v>0.03551591999999881</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -2854,13 +2854,13 @@
         <v>37970</v>
       </c>
       <c r="B168">
-        <v>1032542.279999999</v>
+        <v>1032542.28</v>
       </c>
       <c r="C168" s="1">
         <v>-0.00287165068403783</v>
       </c>
       <c r="D168" s="1">
-        <v>0.03254227999999837</v>
+        <v>0.03254227999999881</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -2874,7 +2874,7 @@
         <v>0.004824344820049564</v>
       </c>
       <c r="D169" s="1">
-        <v>0.03752361999999843</v>
+        <v>0.03752361999999887</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -2882,13 +2882,13 @@
         <v>37972</v>
       </c>
       <c r="B170">
-        <v>1039623.449999999</v>
+        <v>1039623.45</v>
       </c>
       <c r="C170" s="1">
         <v>0.002023886453784929</v>
       </c>
       <c r="D170" s="1">
-        <v>0.03962344999999834</v>
+        <v>0.03962344999999878</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -2896,13 +2896,13 @@
         <v>37973</v>
       </c>
       <c r="B171">
-        <v>1047566.319999999</v>
+        <v>1047566.32</v>
       </c>
       <c r="C171" s="1">
         <v>0.007640141245371046</v>
       </c>
       <c r="D171" s="1">
-        <v>0.04756631999999827</v>
+        <v>0.04756631999999872</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -2910,13 +2910,13 @@
         <v>37974</v>
       </c>
       <c r="B172">
-        <v>1047264.739999999</v>
+        <v>1047264.74</v>
       </c>
       <c r="C172" s="1">
         <v>-0.0002878863077614424</v>
       </c>
       <c r="D172" s="1">
-        <v>0.04726473999999814</v>
+        <v>0.04726473999999858</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -2924,13 +2924,13 @@
         <v>37975</v>
       </c>
       <c r="B173">
-        <v>1047264.739999999</v>
+        <v>1047264.74</v>
       </c>
       <c r="C173" s="1">
         <v>0</v>
       </c>
       <c r="D173" s="1">
-        <v>0.04726473999999814</v>
+        <v>0.04726473999999858</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -2938,13 +2938,13 @@
         <v>37976</v>
       </c>
       <c r="B174">
-        <v>1047264.739999999</v>
+        <v>1047264.74</v>
       </c>
       <c r="C174" s="1">
         <v>0</v>
       </c>
       <c r="D174" s="1">
-        <v>0.04726473999999814</v>
+        <v>0.04726473999999858</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -2952,13 +2952,13 @@
         <v>37977</v>
       </c>
       <c r="B175">
-        <v>1049726.609999999</v>
+        <v>1049726.61</v>
       </c>
       <c r="C175" s="1">
         <v>0.002350761852251582</v>
       </c>
       <c r="D175" s="1">
-        <v>0.04972660999999823</v>
+        <v>0.04972660999999867</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -2972,7 +2972,7 @@
         <v>0.002444169725296597</v>
       </c>
       <c r="D176" s="1">
-        <v>0.0522923199999985</v>
+        <v>0.05229231999999895</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -2986,7 +2986,7 @@
         <v>-0.0004066550633001764</v>
       </c>
       <c r="D177" s="1">
-        <v>0.05186439999999859</v>
+        <v>0.05186439999999903</v>
       </c>
     </row>
     <row r="178" spans="1:4">
@@ -3000,7 +3000,7 @@
         <v>0</v>
       </c>
       <c r="D178" s="1">
-        <v>0.05186439999999859</v>
+        <v>0.05186439999999903</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -3011,10 +3011,10 @@
         <v>1052846.49</v>
       </c>
       <c r="C179" s="1">
-        <v>0.0009336659744354492</v>
+        <v>0.0009336659744356712</v>
       </c>
       <c r="D179" s="1">
-        <v>0.05284648999999852</v>
+        <v>0.05284648999999919</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -3028,7 +3028,7 @@
         <v>0</v>
       </c>
       <c r="D180" s="1">
-        <v>0.05284648999999852</v>
+        <v>0.05284648999999919</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -3042,7 +3042,7 @@
         <v>0</v>
       </c>
       <c r="D181" s="1">
-        <v>0.05284648999999852</v>
+        <v>0.05284648999999919</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -3053,10 +3053,10 @@
         <v>1062515.84</v>
       </c>
       <c r="C182" s="1">
-        <v>0.009184007442528674</v>
+        <v>0.009184007442528452</v>
       </c>
       <c r="D182" s="1">
-        <v>0.06251583999999877</v>
+        <v>0.06251583999999921</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -3070,7 +3070,7 @@
         <v>0.001106919968365094</v>
       </c>
       <c r="D183" s="1">
-        <v>0.06369195999999899</v>
+        <v>0.06369195999999944</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -3084,7 +3084,7 @@
         <v>0.001265121906157907</v>
       </c>
       <c r="D184" s="1">
-        <v>0.06503765999999911</v>
+        <v>0.06503765999999955</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -3098,7 +3098,7 @@
         <v>0</v>
       </c>
       <c r="D185" s="1">
-        <v>0.06503765999999911</v>
+        <v>0.06503765999999955</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -3112,7 +3112,7 @@
         <v>-0.0004269520384847514</v>
       </c>
       <c r="D186" s="1">
-        <v>0.06458293999999909</v>
+        <v>0.06458293999999953</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -3126,7 +3126,7 @@
         <v>0</v>
       </c>
       <c r="D187" s="1">
-        <v>0.06458293999999909</v>
+        <v>0.06458293999999953</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -3140,7 +3140,7 @@
         <v>0</v>
       </c>
       <c r="D188" s="1">
-        <v>0.06458293999999909</v>
+        <v>0.06458293999999953</v>
       </c>
     </row>
     <row r="189" spans="1:4">
@@ -3151,10 +3151,10 @@
         <v>1070456.91</v>
       </c>
       <c r="C189" s="1">
-        <v>0.005517625521972214</v>
+        <v>0.005517625521971992</v>
       </c>
       <c r="D189" s="1">
-        <v>0.07045690999999921</v>
+        <v>0.07045690999999943</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -3168,7 +3168,7 @@
         <v>0.0008927683039572365</v>
       </c>
       <c r="D190" s="1">
-        <v>0.07141257999999917</v>
+        <v>0.07141257999999939</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -3182,7 +3182,7 @@
         <v>0.002863649407588431</v>
       </c>
       <c r="D191" s="1">
-        <v>0.074480729999999</v>
+        <v>0.07448072999999922</v>
       </c>
     </row>
     <row r="192" spans="1:4">
@@ -3196,7 +3196,7 @@
         <v>0.0002941606965813914</v>
       </c>
       <c r="D192" s="1">
-        <v>0.074796799999999</v>
+        <v>0.07479679999999922</v>
       </c>
     </row>
     <row r="193" spans="1:4">
@@ -3210,7 +3210,7 @@
         <v>-0.006712059433001571</v>
       </c>
       <c r="D193" s="1">
-        <v>0.06758269999999911</v>
+        <v>0.06758269999999933</v>
       </c>
     </row>
     <row r="194" spans="1:4">
@@ -3224,7 +3224,7 @@
         <v>0</v>
       </c>
       <c r="D194" s="1">
-        <v>0.06758269999999911</v>
+        <v>0.06758269999999933</v>
       </c>
     </row>
     <row r="195" spans="1:4">
@@ -3238,7 +3238,7 @@
         <v>0</v>
       </c>
       <c r="D195" s="1">
-        <v>0.06758269999999911</v>
+        <v>0.06758269999999933</v>
       </c>
     </row>
     <row r="196" spans="1:4">
@@ -3249,10 +3249,10 @@
         <v>1069404.9</v>
       </c>
       <c r="C196" s="1">
-        <v>0.001706846692064001</v>
+        <v>0.001706846692064223</v>
       </c>
       <c r="D196" s="1">
-        <v>0.06940489999999877</v>
+        <v>0.06940489999999921</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -3263,10 +3263,10 @@
         <v>1066170.9</v>
       </c>
       <c r="C197" s="1">
-        <v>-0.003024111821443909</v>
+        <v>-0.003024111821443687</v>
       </c>
       <c r="D197" s="1">
-        <v>0.06617089999999881</v>
+        <v>0.06617089999999948</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -3277,10 +3277,10 @@
         <v>1073065.8</v>
       </c>
       <c r="C198" s="1">
-        <v>0.00646697447848199</v>
+        <v>0.006466974478481768</v>
       </c>
       <c r="D198" s="1">
-        <v>0.07306579999999907</v>
+        <v>0.07306579999999951</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -3291,10 +3291,10 @@
         <v>1072827.49</v>
       </c>
       <c r="C199" s="1">
-        <v>-0.0002220833056091331</v>
+        <v>-0.0002220833056089111</v>
       </c>
       <c r="D199" s="1">
-        <v>0.072827489999999</v>
+        <v>0.07282748999999966</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -3305,10 +3305,10 @@
         <v>1076057.14</v>
       </c>
       <c r="C200" s="1">
-        <v>0.003010409436842609</v>
+        <v>0.003010409436842165</v>
       </c>
       <c r="D200" s="1">
-        <v>0.07605713999999919</v>
+        <v>0.07605713999999941</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -3322,7 +3322,7 @@
         <v>0</v>
       </c>
       <c r="D201" s="1">
-        <v>0.07605713999999919</v>
+        <v>0.07605713999999941</v>
       </c>
     </row>
     <row r="202" spans="1:4">
@@ -3336,7 +3336,7 @@
         <v>0</v>
       </c>
       <c r="D202" s="1">
-        <v>0.07605713999999919</v>
+        <v>0.07605713999999941</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -3350,7 +3350,7 @@
         <v>0</v>
       </c>
       <c r="D203" s="1">
-        <v>0.07605713999999919</v>
+        <v>0.07605713999999941</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -3361,10 +3361,10 @@
         <v>1075725.58</v>
       </c>
       <c r="C204" s="1">
-        <v>-0.000308124901248541</v>
+        <v>-0.0003081249012480969</v>
       </c>
       <c r="D204" s="1">
-        <v>0.07572557999999896</v>
+        <v>0.07572557999999963</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -3372,13 +3372,13 @@
         <v>38007</v>
       </c>
       <c r="B205">
-        <v>1085490.119999999</v>
+        <v>1085490.12</v>
       </c>
       <c r="C205" s="1">
-        <v>0.009077166315966778</v>
+        <v>0.009077166315967</v>
       </c>
       <c r="D205" s="1">
-        <v>0.08549011999999867</v>
+        <v>0.08549011999999978</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -3386,13 +3386,13 @@
         <v>38008</v>
       </c>
       <c r="B206">
-        <v>1084432.319999999</v>
+        <v>1084432.32</v>
       </c>
       <c r="C206" s="1">
         <v>-0.0009744906752352511</v>
       </c>
       <c r="D206" s="1">
-        <v>0.08443231999999878</v>
+        <v>0.08443231999999989</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -3400,13 +3400,13 @@
         <v>38009</v>
       </c>
       <c r="B207">
-        <v>1083577.949999999</v>
+        <v>1083577.95</v>
       </c>
       <c r="C207" s="1">
         <v>-0.0007878499969458108</v>
       </c>
       <c r="D207" s="1">
-        <v>0.0835779499999989</v>
+        <v>0.08357795000000001</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -3414,13 +3414,13 @@
         <v>38010</v>
       </c>
       <c r="B208">
-        <v>1083577.949999999</v>
+        <v>1083577.95</v>
       </c>
       <c r="C208" s="1">
         <v>0</v>
       </c>
       <c r="D208" s="1">
-        <v>0.0835779499999989</v>
+        <v>0.08357795000000001</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -3428,13 +3428,13 @@
         <v>38011</v>
       </c>
       <c r="B209">
-        <v>1083577.949999999</v>
+        <v>1083577.95</v>
       </c>
       <c r="C209" s="1">
         <v>0</v>
       </c>
       <c r="D209" s="1">
-        <v>0.0835779499999989</v>
+        <v>0.08357795000000001</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -3442,13 +3442,13 @@
         <v>38012</v>
       </c>
       <c r="B210">
-        <v>1092656.959999999</v>
+        <v>1092656.96</v>
       </c>
       <c r="C210" s="1">
-        <v>0.008378732697541524</v>
+        <v>0.008378732697541746</v>
       </c>
       <c r="D210" s="1">
-        <v>0.0926569599999989</v>
+        <v>0.09265696000000023</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -3456,13 +3456,13 @@
         <v>38013</v>
       </c>
       <c r="B211">
-        <v>1085512.99</v>
+        <v>1085512.990000001</v>
       </c>
       <c r="C211" s="1">
-        <v>-0.006538163633717176</v>
+        <v>-0.006538163633716954</v>
       </c>
       <c r="D211" s="1">
-        <v>0.0855129899999989</v>
+        <v>0.08551299000000046</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -3470,13 +3470,13 @@
         <v>38014</v>
       </c>
       <c r="B212">
-        <v>1077676.54</v>
+        <v>1077676.540000001</v>
       </c>
       <c r="C212" s="1">
-        <v>-0.007219121348331137</v>
+        <v>-0.007219121348331359</v>
       </c>
       <c r="D212" s="1">
-        <v>0.07767653999999924</v>
+        <v>0.07767654000000035</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -3484,13 +3484,13 @@
         <v>38015</v>
       </c>
       <c r="B213">
-        <v>1086810.19</v>
+        <v>1086810.190000001</v>
       </c>
       <c r="C213" s="1">
-        <v>0.008475316721657578</v>
+        <v>0.008475316721657356</v>
       </c>
       <c r="D213" s="1">
-        <v>0.08681018999999934</v>
+        <v>0.08681019000000023</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -3498,13 +3498,13 @@
         <v>38016</v>
       </c>
       <c r="B214">
-        <v>1082721</v>
+        <v>1082721.000000001</v>
       </c>
       <c r="C214" s="1">
         <v>-0.00376256133557229</v>
       </c>
       <c r="D214" s="1">
-        <v>0.08272099999999938</v>
+        <v>0.08272100000000027</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -3512,13 +3512,13 @@
         <v>38017</v>
       </c>
       <c r="B215">
-        <v>1082721</v>
+        <v>1082721.000000001</v>
       </c>
       <c r="C215" s="1">
         <v>0</v>
       </c>
       <c r="D215" s="1">
-        <v>0.08272099999999938</v>
+        <v>0.08272100000000027</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -3526,13 +3526,13 @@
         <v>38018</v>
       </c>
       <c r="B216">
-        <v>1082721</v>
+        <v>1082721.000000001</v>
       </c>
       <c r="C216" s="1">
         <v>0</v>
       </c>
       <c r="D216" s="1">
-        <v>0.08272099999999938</v>
+        <v>0.08272100000000027</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -3540,13 +3540,13 @@
         <v>38019</v>
       </c>
       <c r="B217">
-        <v>1088521.56</v>
+        <v>1088521.560000001</v>
       </c>
       <c r="C217" s="1">
         <v>0.005357391239294129</v>
       </c>
       <c r="D217" s="1">
-        <v>0.08852155999999911</v>
+        <v>0.08852156</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -3554,13 +3554,13 @@
         <v>38020</v>
       </c>
       <c r="B218">
-        <v>1091701.88</v>
+        <v>1091701.880000001</v>
       </c>
       <c r="C218" s="1">
         <v>0.002921687651276317</v>
       </c>
       <c r="D218" s="1">
-        <v>0.09170187999999913</v>
+        <v>0.09170188000000001</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -3568,13 +3568,13 @@
         <v>38021</v>
       </c>
       <c r="B219">
-        <v>1090073.58</v>
+        <v>1090073.580000001</v>
       </c>
       <c r="C219" s="1">
-        <v>-0.001491524407743805</v>
+        <v>-0.001491524407744027</v>
       </c>
       <c r="D219" s="1">
-        <v>0.09007357999999943</v>
+        <v>0.09007357999999988</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -3585,10 +3585,10 @@
         <v>1090672.64</v>
       </c>
       <c r="C220" s="1">
-        <v>0.0005495592325062137</v>
+        <v>0.0005495592325059917</v>
       </c>
       <c r="D220" s="1">
-        <v>0.09067263999999953</v>
+        <v>0.09067263999999975</v>
       </c>
     </row>
     <row r="221" spans="1:4">
@@ -3599,10 +3599,10 @@
         <v>1099478.22</v>
       </c>
       <c r="C221" s="1">
-        <v>0.00807353157772428</v>
+        <v>0.008073531577724502</v>
       </c>
       <c r="D221" s="1">
-        <v>0.09947821999999951</v>
+        <v>0.09947821999999995</v>
       </c>
     </row>
     <row r="222" spans="1:4">
@@ -3616,7 +3616,7 @@
         <v>0</v>
       </c>
       <c r="D222" s="1">
-        <v>0.09947821999999951</v>
+        <v>0.09947821999999995</v>
       </c>
     </row>
     <row r="223" spans="1:4">
@@ -3630,7 +3630,7 @@
         <v>0</v>
       </c>
       <c r="D223" s="1">
-        <v>0.09947821999999951</v>
+        <v>0.09947821999999995</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -3638,13 +3638,13 @@
         <v>38026</v>
       </c>
       <c r="B224">
-        <v>1096858.79</v>
+        <v>1096858.790000001</v>
       </c>
       <c r="C224" s="1">
         <v>-0.002382430094886256</v>
       </c>
       <c r="D224" s="1">
-        <v>0.09685878999999953</v>
+        <v>0.09685878999999997</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -3652,13 +3652,13 @@
         <v>38027</v>
       </c>
       <c r="B225">
-        <v>1101318.64</v>
+        <v>1101318.640000001</v>
       </c>
       <c r="C225" s="1">
-        <v>0.004066020203019827</v>
+        <v>0.004066020203020049</v>
       </c>
       <c r="D225" s="1">
-        <v>0.1013186399999995</v>
+        <v>0.1013186400000001</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -3666,13 +3666,13 @@
         <v>38028</v>
       </c>
       <c r="B226">
-        <v>1108022.96</v>
+        <v>1108022.960000001</v>
       </c>
       <c r="C226" s="1">
-        <v>0.006087538843435825</v>
+        <v>0.006087538843436047</v>
       </c>
       <c r="D226" s="1">
-        <v>0.1080229599999993</v>
+        <v>0.1080229600000002</v>
       </c>
     </row>
     <row r="227" spans="1:4">
@@ -3680,13 +3680,13 @@
         <v>38029</v>
       </c>
       <c r="B227">
-        <v>1104228.13</v>
+        <v>1104228.130000001</v>
       </c>
       <c r="C227" s="1">
-        <v>-0.003424865852960202</v>
+        <v>-0.003424865852960424</v>
       </c>
       <c r="D227" s="1">
-        <v>0.1042281299999994</v>
+        <v>0.1042281300000001</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -3700,7 +3700,7 @@
         <v>-0.004374186699989346</v>
       </c>
       <c r="D228" s="1">
-        <v>0.09939802999999925</v>
+        <v>0.09939802999999992</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -3714,7 +3714,7 @@
         <v>0</v>
       </c>
       <c r="D229" s="1">
-        <v>0.09939802999999925</v>
+        <v>0.09939802999999992</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -3728,7 +3728,7 @@
         <v>0</v>
       </c>
       <c r="D230" s="1">
-        <v>0.09939802999999925</v>
+        <v>0.09939802999999992</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -3742,7 +3742,7 @@
         <v>0</v>
       </c>
       <c r="D231" s="1">
-        <v>0.09939802999999925</v>
+        <v>0.09939802999999992</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -3750,13 +3750,13 @@
         <v>38034</v>
       </c>
       <c r="B232">
-        <v>1107054.73</v>
+        <v>1107054.730000001</v>
       </c>
       <c r="C232" s="1">
         <v>0.006964447625943171</v>
       </c>
       <c r="D232" s="1">
-        <v>0.1070547299999993</v>
+        <v>0.10705473</v>
       </c>
     </row>
     <row r="233" spans="1:4">
@@ -3764,13 +3764,13 @@
         <v>38035</v>
       </c>
       <c r="B233">
-        <v>1103918.38</v>
+        <v>1103918.380000001</v>
       </c>
       <c r="C233" s="1">
         <v>-0.002833057765807223</v>
       </c>
       <c r="D233" s="1">
-        <v>0.1039183799999992</v>
+        <v>0.1039183799999999</v>
       </c>
     </row>
     <row r="234" spans="1:4">
@@ -3778,13 +3778,13 @@
         <v>38036</v>
       </c>
       <c r="B234">
-        <v>1102641.62</v>
+        <v>1102641.620000001</v>
       </c>
       <c r="C234" s="1">
         <v>-0.001156571013882446</v>
       </c>
       <c r="D234" s="1">
-        <v>0.1026416199999991</v>
+        <v>0.1026416199999998</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -3792,13 +3792,13 @@
         <v>38037</v>
       </c>
       <c r="B235">
-        <v>1102079.82</v>
+        <v>1102079.820000001</v>
       </c>
       <c r="C235" s="1">
         <v>-0.0005095037134550395</v>
       </c>
       <c r="D235" s="1">
-        <v>0.102079819999999</v>
+        <v>0.1020798199999997</v>
       </c>
     </row>
     <row r="236" spans="1:4">
@@ -3806,13 +3806,13 @@
         <v>38038</v>
       </c>
       <c r="B236">
-        <v>1102079.82</v>
+        <v>1102079.820000001</v>
       </c>
       <c r="C236" s="1">
         <v>0</v>
       </c>
       <c r="D236" s="1">
-        <v>0.102079819999999</v>
+        <v>0.1020798199999997</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -3820,13 +3820,13 @@
         <v>38039</v>
       </c>
       <c r="B237">
-        <v>1102079.82</v>
+        <v>1102079.820000001</v>
       </c>
       <c r="C237" s="1">
         <v>0</v>
       </c>
       <c r="D237" s="1">
-        <v>0.102079819999999</v>
+        <v>0.1020798199999997</v>
       </c>
     </row>
     <row r="238" spans="1:4">
@@ -3834,13 +3834,13 @@
         <v>38040</v>
       </c>
       <c r="B238">
-        <v>1101505.57</v>
+        <v>1101505.570000001</v>
       </c>
       <c r="C238" s="1">
-        <v>-0.0005210602622233163</v>
+        <v>-0.0005210602622230942</v>
       </c>
       <c r="D238" s="1">
-        <v>0.1015055699999987</v>
+        <v>0.1015055699999998</v>
       </c>
     </row>
     <row r="239" spans="1:4">
@@ -3854,7 +3854,7 @@
         <v>-0.001109663022403118</v>
       </c>
       <c r="D239" s="1">
-        <v>0.1002832699999987</v>
+        <v>0.1002832699999998</v>
       </c>
     </row>
     <row r="240" spans="1:4">
@@ -3865,10 +3865,10 @@
         <v>1103377.17</v>
       </c>
       <c r="C240" s="1">
-        <v>0.002811912245107795</v>
+        <v>0.002811912245107573</v>
       </c>
       <c r="D240" s="1">
-        <v>0.103377169999999</v>
+        <v>0.1033771699999999</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -3882,7 +3882,7 @@
         <v>0.0005284684293405117</v>
       </c>
       <c r="D241" s="1">
-        <v>0.1039602699999991</v>
+        <v>0.10396027</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -3896,7 +3896,7 @@
         <v>0.0003718612083747352</v>
       </c>
       <c r="D242" s="1">
-        <v>0.104370789999999</v>
+        <v>0.1043707899999999</v>
       </c>
     </row>
     <row r="243" spans="1:4">
@@ -3910,7 +3910,7 @@
         <v>0</v>
       </c>
       <c r="D243" s="1">
-        <v>0.104370789999999</v>
+        <v>0.1043707899999999</v>
       </c>
     </row>
     <row r="244" spans="1:4">
@@ -3924,7 +3924,7 @@
         <v>0</v>
       </c>
       <c r="D244" s="1">
-        <v>0.104370789999999</v>
+        <v>0.1043707899999999</v>
       </c>
     </row>
     <row r="245" spans="1:4">
@@ -3938,7 +3938,7 @@
         <v>0.007342552042688411</v>
       </c>
       <c r="D245" s="1">
-        <v>0.1124796899999989</v>
+        <v>0.1124796899999998</v>
       </c>
     </row>
     <row r="246" spans="1:4">
@@ -3952,7 +3952,7 @@
         <v>-0.005862614894119988</v>
       </c>
       <c r="D246" s="1">
-        <v>0.105957649999999</v>
+        <v>0.1059576499999999</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -3966,7 +3966,7 @@
         <v>0.002730131664625768</v>
       </c>
       <c r="D247" s="1">
-        <v>0.1089770599999991</v>
+        <v>0.10897706</v>
       </c>
     </row>
     <row r="248" spans="1:4">
@@ -3980,7 +3980,7 @@
         <v>0.001987444176708264</v>
       </c>
       <c r="D248" s="1">
-        <v>0.1111810899999992</v>
+        <v>0.1111810900000001</v>
       </c>
     </row>
     <row r="249" spans="1:4">
@@ -3991,10 +3991,10 @@
         <v>1114084.93</v>
       </c>
       <c r="C249" s="1">
-        <v>0.002613291412293606</v>
+        <v>0.002613291412293384</v>
       </c>
       <c r="D249" s="1">
-        <v>0.1140849299999993</v>
+        <v>0.11408493</v>
       </c>
     </row>
     <row r="250" spans="1:4">
@@ -4008,7 +4008,7 @@
         <v>0</v>
       </c>
       <c r="D250" s="1">
-        <v>0.1140849299999993</v>
+        <v>0.11408493</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -4022,7 +4022,7 @@
         <v>0</v>
       </c>
       <c r="D251" s="1">
-        <v>0.1140849299999993</v>
+        <v>0.11408493</v>
       </c>
     </row>
     <row r="252" spans="1:4">
@@ -4036,7 +4036,7 @@
         <v>-0.003467320933961404</v>
       </c>
       <c r="D252" s="1">
-        <v>0.1102220399999994</v>
+        <v>0.11022204</v>
       </c>
     </row>
     <row r="253" spans="1:4">
@@ -4050,7 +4050,7 @@
         <v>-0.003921359730887808</v>
       </c>
       <c r="D253" s="1">
-        <v>0.1058684599999993</v>
+        <v>0.1058684599999999</v>
       </c>
     </row>
     <row r="254" spans="1:4">
@@ -4064,7 +4064,7 @@
         <v>-0.01018905087500188</v>
       </c>
       <c r="D254" s="1">
-        <v>0.09460070999999926</v>
+        <v>0.09460070999999992</v>
       </c>
     </row>
     <row r="255" spans="1:4">
@@ -4078,7 +4078,7 @@
         <v>-0.01426725732710332</v>
       </c>
       <c r="D255" s="1">
-        <v>0.07898375999999918</v>
+        <v>0.07898375999999985</v>
       </c>
     </row>
     <row r="256" spans="1:4">
@@ -4092,7 +4092,7 @@
         <v>0.006554445268017961</v>
       </c>
       <c r="D256" s="1">
-        <v>0.08605589999999941</v>
+        <v>0.08605590000000007</v>
       </c>
     </row>
     <row r="257" spans="1:4">
@@ -4106,7 +4106,7 @@
         <v>0</v>
       </c>
       <c r="D257" s="1">
-        <v>0.08605589999999941</v>
+        <v>0.08605590000000007</v>
       </c>
     </row>
     <row r="258" spans="1:4">
@@ -4120,7 +4120,7 @@
         <v>0</v>
       </c>
       <c r="D258" s="1">
-        <v>0.08605589999999941</v>
+        <v>0.08605590000000007</v>
       </c>
     </row>
     <row r="259" spans="1:4">
@@ -4131,10 +4131,10 @@
         <v>1075825.72</v>
       </c>
       <c r="C259" s="1">
-        <v>-0.009419570392279253</v>
+        <v>-0.009419570392279031</v>
       </c>
       <c r="D259" s="1">
-        <v>0.07582571999999921</v>
+        <v>0.0758257200000001</v>
       </c>
     </row>
     <row r="260" spans="1:4">
@@ -4145,10 +4145,10 @@
         <v>1080118.76</v>
       </c>
       <c r="C260" s="1">
-        <v>0.00399046046231355</v>
+        <v>0.003990460462313328</v>
       </c>
       <c r="D260" s="1">
-        <v>0.08011875999999929</v>
+        <v>0.08011875999999996</v>
       </c>
     </row>
     <row r="261" spans="1:4">
@@ -4159,10 +4159,10 @@
         <v>1089780.38</v>
       </c>
       <c r="C261" s="1">
-        <v>0.00894496083004781</v>
+        <v>0.008944960830048032</v>
       </c>
       <c r="D261" s="1">
-        <v>0.08978037999999899</v>
+        <v>0.0897803800000001</v>
       </c>
     </row>
     <row r="262" spans="1:4">
@@ -4173,10 +4173,10 @@
         <v>1088421.41</v>
       </c>
       <c r="C262" s="1">
-        <v>-0.001247012723793017</v>
+        <v>-0.001247012723793239</v>
       </c>
       <c r="D262" s="1">
-        <v>0.08842140999999892</v>
+        <v>0.08842140999999981</v>
       </c>
     </row>
     <row r="263" spans="1:4">
@@ -4187,10 +4187,10 @@
         <v>1079960.16</v>
       </c>
       <c r="C263" s="1">
-        <v>-0.007773873172891688</v>
+        <v>-0.00777387317289191</v>
       </c>
       <c r="D263" s="1">
-        <v>0.07996015999999906</v>
+        <v>0.07996015999999972</v>
       </c>
     </row>
     <row r="264" spans="1:4">
@@ -4204,7 +4204,7 @@
         <v>0</v>
       </c>
       <c r="D264" s="1">
-        <v>0.07996015999999906</v>
+        <v>0.07996015999999972</v>
       </c>
     </row>
     <row r="265" spans="1:4">
@@ -4218,7 +4218,7 @@
         <v>0</v>
       </c>
       <c r="D265" s="1">
-        <v>0.07996015999999906</v>
+        <v>0.07996015999999972</v>
       </c>
     </row>
     <row r="266" spans="1:4">
@@ -4232,7 +4232,7 @@
         <v>-0.01024651687151135</v>
       </c>
       <c r="D266" s="1">
-        <v>0.06889432999999889</v>
+        <v>0.06889432999999956</v>
       </c>
     </row>
     <row r="267" spans="1:4">
@@ -4246,7 +4246,7 @@
         <v>-0.0003073924061325339</v>
       </c>
       <c r="D267" s="1">
-        <v>0.0685657599999987</v>
+        <v>0.06856575999999936</v>
       </c>
     </row>
     <row r="268" spans="1:4">
@@ -4260,7 +4260,7 @@
         <v>-0.002170114453227345</v>
       </c>
       <c r="D268" s="1">
-        <v>0.06624684999999886</v>
+        <v>0.06624684999999952</v>
       </c>
     </row>
     <row r="269" spans="1:4">
@@ -4274,7 +4274,7 @@
         <v>0.0101121705541265</v>
       </c>
       <c r="D269" s="1">
-        <v>0.07702891999999895</v>
+        <v>0.07702891999999961</v>
       </c>
     </row>
     <row r="270" spans="1:4">
@@ -4288,7 +4288,7 @@
         <v>-0.0009831955115930935</v>
       </c>
       <c r="D270" s="1">
-        <v>0.07596998999999904</v>
+        <v>0.07596998999999971</v>
       </c>
     </row>
     <row r="271" spans="1:4">
@@ -4302,7 +4302,7 @@
         <v>0</v>
       </c>
       <c r="D271" s="1">
-        <v>0.07596998999999904</v>
+        <v>0.07596998999999971</v>
       </c>
     </row>
     <row r="272" spans="1:4">
@@ -4316,7 +4316,7 @@
         <v>0</v>
       </c>
       <c r="D272" s="1">
-        <v>0.07596998999999904</v>
+        <v>0.07596998999999971</v>
       </c>
     </row>
     <row r="273" spans="1:4">
@@ -4330,7 +4330,7 @@
         <v>0.01071520591387487</v>
       </c>
       <c r="D273" s="1">
-        <v>0.08749922999999882</v>
+        <v>0.08749922999999948</v>
       </c>
     </row>
     <row r="274" spans="1:4">
@@ -4341,10 +4341,10 @@
         <v>1090742.97</v>
       </c>
       <c r="C274" s="1">
-        <v>0.002982751537212724</v>
+        <v>0.00298275153721228</v>
       </c>
       <c r="D274" s="1">
-        <v>0.09074296999999887</v>
+        <v>0.09074296999999909</v>
       </c>
     </row>
     <row r="275" spans="1:4">
@@ -4358,7 +4358,7 @@
         <v>0.0004874658967546353</v>
       </c>
       <c r="D275" s="1">
-        <v>0.09127466999999867</v>
+        <v>0.09127466999999889</v>
       </c>
     </row>
     <row r="276" spans="1:4">
@@ -4369,7 +4369,7 @@
         <v>1095673.88</v>
       </c>
       <c r="C276" s="1">
-        <v>0.004031258234922896</v>
+        <v>0.004031258234922674</v>
       </c>
       <c r="D276" s="1">
         <v>0.09567387999999899</v>
@@ -4383,10 +4383,10 @@
         <v>1101000.3</v>
       </c>
       <c r="C277" s="1">
-        <v>0.004861318771238521</v>
+        <v>0.004861318771238743</v>
       </c>
       <c r="D277" s="1">
-        <v>0.1010002999999988</v>
+        <v>0.101000299999999</v>
       </c>
     </row>
     <row r="278" spans="1:4">
@@ -4400,7 +4400,7 @@
         <v>0</v>
       </c>
       <c r="D278" s="1">
-        <v>0.1010002999999988</v>
+        <v>0.101000299999999</v>
       </c>
     </row>
     <row r="279" spans="1:4">
@@ -4414,7 +4414,7 @@
         <v>0</v>
       </c>
       <c r="D279" s="1">
-        <v>0.1010002999999988</v>
+        <v>0.101000299999999</v>
       </c>
     </row>
     <row r="280" spans="1:4">
@@ -4428,7 +4428,7 @@
         <v>0.006227455160548345</v>
       </c>
       <c r="D280" s="1">
-        <v>0.1078567299999991</v>
+        <v>0.1078567299999993</v>
       </c>
     </row>
     <row r="281" spans="1:4">
@@ -4442,7 +4442,7 @@
         <v>-7.040621579312845E-05</v>
       </c>
       <c r="D281" s="1">
-        <v>0.1077787299999988</v>
+        <v>0.107778729999999</v>
       </c>
     </row>
     <row r="282" spans="1:4">
@@ -4453,10 +4453,10 @@
         <v>1101178.94</v>
       </c>
       <c r="C282" s="1">
-        <v>-0.00595767893106236</v>
+        <v>-0.005957678931062138</v>
       </c>
       <c r="D282" s="1">
-        <v>0.1011789399999987</v>
+        <v>0.1011789399999994</v>
       </c>
     </row>
     <row r="283" spans="1:4">
@@ -4470,7 +4470,7 @@
         <v>-0.003572289531799444</v>
       </c>
       <c r="D283" s="1">
-        <v>0.09724520999999875</v>
+        <v>0.09724520999999942</v>
       </c>
     </row>
     <row r="284" spans="1:4">
@@ -4484,7 +4484,7 @@
         <v>0</v>
       </c>
       <c r="D284" s="1">
-        <v>0.09724520999999875</v>
+        <v>0.09724520999999942</v>
       </c>
     </row>
     <row r="285" spans="1:4">
@@ -4498,7 +4498,7 @@
         <v>0</v>
       </c>
       <c r="D285" s="1">
-        <v>0.09724520999999875</v>
+        <v>0.09724520999999942</v>
       </c>
     </row>
     <row r="286" spans="1:4">
@@ -4512,7 +4512,7 @@
         <v>0</v>
       </c>
       <c r="D286" s="1">
-        <v>0.09724520999999875</v>
+        <v>0.09724520999999942</v>
       </c>
     </row>
     <row r="287" spans="1:4">
@@ -4523,10 +4523,10 @@
         <v>1098252.33</v>
       </c>
       <c r="C287" s="1">
-        <v>0.0009178622889589594</v>
+        <v>0.0009178622889591814</v>
       </c>
       <c r="D287" s="1">
-        <v>0.09825232999999867</v>
+        <v>0.09825232999999955</v>
       </c>
     </row>
     <row r="288" spans="1:4">
@@ -4537,10 +4537,10 @@
         <v>1085414.41</v>
       </c>
       <c r="C288" s="1">
-        <v>-0.01168940838941823</v>
+        <v>-0.01168940838941801</v>
       </c>
       <c r="D288" s="1">
-        <v>0.0854144099999985</v>
+        <v>0.08541440999999961</v>
       </c>
     </row>
     <row r="289" spans="1:4">
@@ -4551,10 +4551,10 @@
         <v>1088927.77</v>
       </c>
       <c r="C289" s="1">
-        <v>0.003236883505167265</v>
+        <v>0.003236883505167487</v>
       </c>
       <c r="D289" s="1">
-        <v>0.08892776999999841</v>
+        <v>0.08892776999999974</v>
       </c>
     </row>
     <row r="290" spans="1:4">
@@ -4568,7 +4568,7 @@
         <v>0.008122834446586014</v>
       </c>
       <c r="D290" s="1">
-        <v>0.09777294999999842</v>
+        <v>0.09777294999999975</v>
       </c>
     </row>
     <row r="291" spans="1:4">
@@ -4579,10 +4579,10 @@
         <v>1104490.14</v>
       </c>
       <c r="C291" s="1">
-        <v>0.006118924682922966</v>
+        <v>0.006118924682922744</v>
       </c>
       <c r="D291" s="1">
-        <v>0.1044901399999985</v>
+        <v>0.1044901399999996</v>
       </c>
     </row>
     <row r="292" spans="1:4">
@@ -4596,7 +4596,7 @@
         <v>0</v>
       </c>
       <c r="D292" s="1">
-        <v>0.1044901399999985</v>
+        <v>0.1044901399999996</v>
       </c>
     </row>
     <row r="293" spans="1:4">
@@ -4610,7 +4610,7 @@
         <v>0</v>
       </c>
       <c r="D293" s="1">
-        <v>0.1044901399999985</v>
+        <v>0.1044901399999996</v>
       </c>
     </row>
     <row r="294" spans="1:4">
@@ -4621,10 +4621,10 @@
         <v>1104321.36</v>
       </c>
       <c r="C294" s="1">
-        <v>-0.0001528125909754374</v>
+        <v>-0.0001528125909752154</v>
       </c>
       <c r="D294" s="1">
-        <v>0.1043213599999981</v>
+        <v>0.1043213599999997</v>
       </c>
     </row>
     <row r="295" spans="1:4">
@@ -4635,10 +4635,10 @@
         <v>1090408.66</v>
       </c>
       <c r="C295" s="1">
-        <v>-0.01259841609873413</v>
+        <v>-0.01259841609873436</v>
       </c>
       <c r="D295" s="1">
-        <v>0.09040865999999825</v>
+        <v>0.09040865999999959</v>
       </c>
     </row>
     <row r="296" spans="1:4">
@@ -4649,10 +4649,10 @@
         <v>1096012.64</v>
       </c>
       <c r="C296" s="1">
-        <v>0.005139339227184792</v>
+        <v>0.005139339227185014</v>
       </c>
       <c r="D296" s="1">
-        <v>0.09601263999999832</v>
+        <v>0.09601263999999987</v>
       </c>
     </row>
     <row r="297" spans="1:4">
@@ -4666,7 +4666,7 @@
         <v>0.01001913627565476</v>
       </c>
       <c r="D297" s="1">
-        <v>0.1069937399999985</v>
+        <v>0.1069937400000001</v>
       </c>
     </row>
     <row r="298" spans="1:4">
@@ -4677,10 +4677,10 @@
         <v>1107082.47</v>
       </c>
       <c r="C298" s="1">
-        <v>8.015402146721584E-05</v>
+        <v>8.01540214669938E-05</v>
       </c>
       <c r="D298" s="1">
-        <v>0.1070824699999986</v>
+        <v>0.1070824699999999</v>
       </c>
     </row>
     <row r="299" spans="1:4">
@@ -4694,7 +4694,7 @@
         <v>0</v>
       </c>
       <c r="D299" s="1">
-        <v>0.1070824699999986</v>
+        <v>0.1070824699999999</v>
       </c>
     </row>
     <row r="300" spans="1:4">
@@ -4708,7 +4708,7 @@
         <v>0</v>
       </c>
       <c r="D300" s="1">
-        <v>0.1070824699999986</v>
+        <v>0.1070824699999999</v>
       </c>
     </row>
     <row r="301" spans="1:4">
@@ -4719,10 +4719,10 @@
         <v>1104895.21</v>
       </c>
       <c r="C301" s="1">
-        <v>-0.001975697438330815</v>
+        <v>-0.001975697438330704</v>
       </c>
       <c r="D301" s="1">
-        <v>0.1048952099999987</v>
+        <v>0.10489521</v>
       </c>
     </row>
     <row r="302" spans="1:4">
@@ -4736,7 +4736,7 @@
         <v>0.002530764885839254</v>
       </c>
       <c r="D302" s="1">
-        <v>0.1076914399999986</v>
+        <v>0.10769144</v>
       </c>
     </row>
     <row r="303" spans="1:4">
@@ -4747,10 +4747,10 @@
         <v>1097710.26</v>
       </c>
       <c r="C303" s="1">
-        <v>-0.009010794558455881</v>
+        <v>-0.009010794558455659</v>
       </c>
       <c r="D303" s="1">
-        <v>0.09771025999999838</v>
+        <v>0.09771026000000016</v>
       </c>
     </row>
     <row r="304" spans="1:4">
@@ -4764,7 +4764,7 @@
         <v>-0.004460411985217294</v>
       </c>
       <c r="D304" s="1">
-        <v>0.0928140199999985</v>
+        <v>0.09281402000000027</v>
       </c>
     </row>
     <row r="305" spans="1:4">
@@ -4778,7 +4778,7 @@
         <v>-0.001610072681900609</v>
       </c>
       <c r="D305" s="1">
-        <v>0.09105450999999842</v>
+        <v>0.0910545100000002</v>
       </c>
     </row>
     <row r="306" spans="1:4">
@@ -4792,7 +4792,7 @@
         <v>0</v>
       </c>
       <c r="D306" s="1">
-        <v>0.09105450999999842</v>
+        <v>0.0910545100000002</v>
       </c>
     </row>
     <row r="307" spans="1:4">
@@ -4806,7 +4806,7 @@
         <v>0</v>
       </c>
       <c r="D307" s="1">
-        <v>0.09105450999999842</v>
+        <v>0.0910545100000002</v>
       </c>
     </row>
     <row r="308" spans="1:4">
@@ -4820,7 +4820,7 @@
         <v>0.008640906493297296</v>
       </c>
       <c r="D308" s="1">
-        <v>0.1004822099999987</v>
+        <v>0.1004822100000005</v>
       </c>
     </row>
     <row r="309" spans="1:4">
@@ -4828,13 +4828,13 @@
         <v>38111</v>
       </c>
       <c r="B309">
-        <v>1100580.1</v>
+        <v>1100580.100000001</v>
       </c>
       <c r="C309" s="1">
-        <v>8.895191499713739E-05</v>
+        <v>8.895191499735944E-05</v>
       </c>
       <c r="D309" s="1">
-        <v>0.1005800999999984</v>
+        <v>0.1005801000000004</v>
       </c>
     </row>
     <row r="310" spans="1:4">
@@ -4842,13 +4842,13 @@
         <v>38112</v>
       </c>
       <c r="B310">
-        <v>1101924.2</v>
+        <v>1101924.200000001</v>
       </c>
       <c r="C310" s="1">
         <v>0.001221265040136643</v>
       </c>
       <c r="D310" s="1">
-        <v>0.1019241999999985</v>
+        <v>0.1019242000000005</v>
       </c>
     </row>
     <row r="311" spans="1:4">
@@ -4859,10 +4859,10 @@
         <v>1098718.77</v>
       </c>
       <c r="C311" s="1">
-        <v>-0.002908938745514345</v>
+        <v>-0.002908938745514567</v>
       </c>
       <c r="D311" s="1">
-        <v>0.09871876999999851</v>
+        <v>0.09871877000000029</v>
       </c>
     </row>
     <row r="312" spans="1:4">
@@ -4876,7 +4876,7 @@
         <v>-0.01145918349970498</v>
       </c>
       <c r="D312" s="1">
-        <v>0.0861283499999983</v>
+        <v>0.08612835000000008</v>
       </c>
     </row>
     <row r="313" spans="1:4">
@@ -4890,7 +4890,7 @@
         <v>0</v>
       </c>
       <c r="D313" s="1">
-        <v>0.0861283499999983</v>
+        <v>0.08612835000000008</v>
       </c>
     </row>
     <row r="314" spans="1:4">
@@ -4904,7 +4904,7 @@
         <v>0</v>
       </c>
       <c r="D314" s="1">
-        <v>0.0861283499999983</v>
+        <v>0.08612835000000008</v>
       </c>
     </row>
     <row r="315" spans="1:4">
@@ -4912,13 +4912,13 @@
         <v>38117</v>
       </c>
       <c r="B315">
-        <v>1075298.449999999</v>
+        <v>1075298.45</v>
       </c>
       <c r="C315" s="1">
-        <v>-0.009971105164504834</v>
+        <v>-0.009971105164504612</v>
       </c>
       <c r="D315" s="1">
-        <v>0.07529844999999824</v>
+        <v>0.07529845000000024</v>
       </c>
     </row>
     <row r="316" spans="1:4">
@@ -4932,7 +4932,7 @@
         <v>0.002092470234658972</v>
       </c>
       <c r="D316" s="1">
-        <v>0.07754847999999814</v>
+        <v>0.07754848000000014</v>
       </c>
     </row>
     <row r="317" spans="1:4">
@@ -4946,7 +4946,7 @@
         <v>0.001044082953928882</v>
       </c>
       <c r="D317" s="1">
-        <v>0.0786735299999981</v>
+        <v>0.0786735300000001</v>
       </c>
     </row>
     <row r="318" spans="1:4">
@@ -4954,13 +4954,13 @@
         <v>38120</v>
       </c>
       <c r="B318">
-        <v>1077373.779999999</v>
+        <v>1077373.78</v>
       </c>
       <c r="C318" s="1">
         <v>-0.001204952160085204</v>
       </c>
       <c r="D318" s="1">
-        <v>0.07737377999999784</v>
+        <v>0.07737377999999984</v>
       </c>
     </row>
     <row r="319" spans="1:4">
@@ -4968,13 +4968,13 @@
         <v>38121</v>
       </c>
       <c r="B319">
-        <v>1079810.059999999</v>
+        <v>1079810.060000001</v>
       </c>
       <c r="C319" s="1">
-        <v>0.002261313617637928</v>
+        <v>0.00226131361763815</v>
       </c>
       <c r="D319" s="1">
-        <v>0.0798100599999978</v>
+        <v>0.07981006000000002</v>
       </c>
     </row>
     <row r="320" spans="1:4">
@@ -4982,13 +4982,13 @@
         <v>38122</v>
       </c>
       <c r="B320">
-        <v>1079810.059999999</v>
+        <v>1079810.060000001</v>
       </c>
       <c r="C320" s="1">
         <v>0</v>
       </c>
       <c r="D320" s="1">
-        <v>0.0798100599999978</v>
+        <v>0.07981006000000002</v>
       </c>
     </row>
     <row r="321" spans="1:4">
@@ -4996,13 +4996,13 @@
         <v>38123</v>
       </c>
       <c r="B321">
-        <v>1079810.059999999</v>
+        <v>1079810.060000001</v>
       </c>
       <c r="C321" s="1">
         <v>0</v>
       </c>
       <c r="D321" s="1">
-        <v>0.0798100599999978</v>
+        <v>0.07981006000000002</v>
       </c>
     </row>
     <row r="322" spans="1:4">
@@ -5013,10 +5013,10 @@
         <v>1071792.75</v>
       </c>
       <c r="C322" s="1">
-        <v>-0.007424740977130528</v>
+        <v>-0.00742474097713075</v>
       </c>
       <c r="D322" s="1">
-        <v>0.07179274999999796</v>
+        <v>0.07179274999999996</v>
       </c>
     </row>
     <row r="323" spans="1:4">
@@ -5024,13 +5024,13 @@
         <v>38125</v>
       </c>
       <c r="B323">
-        <v>1075819.63</v>
+        <v>1075819.630000001</v>
       </c>
       <c r="C323" s="1">
         <v>0.00375714427999263</v>
       </c>
       <c r="D323" s="1">
-        <v>0.07581962999999803</v>
+        <v>0.07581963000000003</v>
       </c>
     </row>
     <row r="324" spans="1:4">
@@ -5044,7 +5044,7 @@
         <v>-0.004866652228682766</v>
       </c>
       <c r="D324" s="1">
-        <v>0.07058398999999782</v>
+        <v>0.07058398999999982</v>
       </c>
     </row>
     <row r="325" spans="1:4">
@@ -5052,13 +5052,13 @@
         <v>38127</v>
       </c>
       <c r="B325">
-        <v>1070324.339999999</v>
+        <v>1070324.34</v>
       </c>
       <c r="C325" s="1">
         <v>-0.000242531181509742</v>
       </c>
       <c r="D325" s="1">
-        <v>0.07032433999999776</v>
+        <v>0.07032433999999976</v>
       </c>
     </row>
     <row r="326" spans="1:4">
@@ -5066,13 +5066,13 @@
         <v>38128</v>
       </c>
       <c r="B326">
-        <v>1072294.819999999</v>
+        <v>1072294.82</v>
       </c>
       <c r="C326" s="1">
         <v>0.001841012043134471</v>
       </c>
       <c r="D326" s="1">
-        <v>0.07229481999999776</v>
+        <v>0.07229481999999976</v>
       </c>
     </row>
     <row r="327" spans="1:4">
@@ -5080,13 +5080,13 @@
         <v>38129</v>
       </c>
       <c r="B327">
-        <v>1072294.819999999</v>
+        <v>1072294.82</v>
       </c>
       <c r="C327" s="1">
         <v>0</v>
       </c>
       <c r="D327" s="1">
-        <v>0.07229481999999776</v>
+        <v>0.07229481999999976</v>
       </c>
     </row>
     <row r="328" spans="1:4">
@@ -5094,13 +5094,13 @@
         <v>38130</v>
       </c>
       <c r="B328">
-        <v>1072294.819999999</v>
+        <v>1072294.82</v>
       </c>
       <c r="C328" s="1">
         <v>0</v>
       </c>
       <c r="D328" s="1">
-        <v>0.07229481999999776</v>
+        <v>0.07229481999999976</v>
       </c>
     </row>
     <row r="329" spans="1:4">
@@ -5108,13 +5108,13 @@
         <v>38131</v>
       </c>
       <c r="B329">
-        <v>1072149.829999999</v>
+        <v>1072149.83</v>
       </c>
       <c r="C329" s="1">
         <v>-0.000135214679112261</v>
       </c>
       <c r="D329" s="1">
-        <v>0.07214982999999764</v>
+        <v>0.07214982999999964</v>
       </c>
     </row>
     <row r="330" spans="1:4">
@@ -5122,13 +5122,13 @@
         <v>38132</v>
       </c>
       <c r="B330">
-        <v>1085827.509999999</v>
+        <v>1085827.51</v>
       </c>
       <c r="C330" s="1">
-        <v>0.01275724681129686</v>
+        <v>0.01275724681129664</v>
       </c>
       <c r="D330" s="1">
-        <v>0.08582750999999766</v>
+        <v>0.08582750999999944</v>
       </c>
     </row>
     <row r="331" spans="1:4">
@@ -5136,13 +5136,13 @@
         <v>38133</v>
       </c>
       <c r="B331">
-        <v>1088066.889999999</v>
+        <v>1088066.89</v>
       </c>
       <c r="C331" s="1">
         <v>0.002062371766579973</v>
       </c>
       <c r="D331" s="1">
-        <v>0.08806688999999746</v>
+        <v>0.08806688999999923</v>
       </c>
     </row>
     <row r="332" spans="1:4">
@@ -5150,13 +5150,13 @@
         <v>38134</v>
       </c>
       <c r="B332">
-        <v>1096773.429999999</v>
+        <v>1096773.43</v>
       </c>
       <c r="C332" s="1">
         <v>0.008001842607305187</v>
       </c>
       <c r="D332" s="1">
-        <v>0.09677342999999738</v>
+        <v>0.09677342999999916</v>
       </c>
     </row>
     <row r="333" spans="1:4">
@@ -5164,13 +5164,13 @@
         <v>38135</v>
       </c>
       <c r="B333">
-        <v>1096122.569999999</v>
+        <v>1096122.57</v>
       </c>
       <c r="C333" s="1">
         <v>-0.0005934315896037878</v>
       </c>
       <c r="D333" s="1">
-        <v>0.09612256999999724</v>
+        <v>0.09612256999999902</v>
       </c>
     </row>
     <row r="334" spans="1:4">
@@ -5178,13 +5178,13 @@
         <v>38136</v>
       </c>
       <c r="B334">
-        <v>1096122.569999999</v>
+        <v>1096122.57</v>
       </c>
       <c r="C334" s="1">
         <v>0</v>
       </c>
       <c r="D334" s="1">
-        <v>0.09612256999999724</v>
+        <v>0.09612256999999902</v>
       </c>
     </row>
     <row r="335" spans="1:4">
@@ -5192,13 +5192,13 @@
         <v>38137</v>
       </c>
       <c r="B335">
-        <v>1096122.569999999</v>
+        <v>1096122.57</v>
       </c>
       <c r="C335" s="1">
         <v>0</v>
       </c>
       <c r="D335" s="1">
-        <v>0.09612256999999724</v>
+        <v>0.09612256999999902</v>
       </c>
     </row>
     <row r="336" spans="1:4">
@@ -5206,13 +5206,13 @@
         <v>38138</v>
       </c>
       <c r="B336">
-        <v>1096122.569999999</v>
+        <v>1096122.57</v>
       </c>
       <c r="C336" s="1">
         <v>0</v>
       </c>
       <c r="D336" s="1">
-        <v>0.09612256999999724</v>
+        <v>0.09612256999999902</v>
       </c>
     </row>
     <row r="337" spans="1:4">
@@ -5220,13 +5220,13 @@
         <v>38139</v>
       </c>
       <c r="B337">
-        <v>1098105.959999999</v>
+        <v>1098105.96</v>
       </c>
       <c r="C337" s="1">
         <v>0.00180946004970961</v>
       </c>
       <c r="D337" s="1">
-        <v>0.09810595999999716</v>
+        <v>0.09810595999999894</v>
       </c>
     </row>
     <row r="338" spans="1:4">
@@ -5234,13 +5234,13 @@
         <v>38140</v>
       </c>
       <c r="B338">
-        <v>1102415.369999999</v>
+        <v>1102415.37</v>
       </c>
       <c r="C338" s="1">
-        <v>0.003924402705181684</v>
+        <v>0.003924402705181462</v>
       </c>
       <c r="D338" s="1">
-        <v>0.1024153699999972</v>
+        <v>0.1024153699999988</v>
       </c>
     </row>
     <row r="339" spans="1:4">
@@ -5254,7 +5254,7 @@
         <v>-0.004100332889952152</v>
       </c>
       <c r="D339" s="1">
-        <v>0.09789509999999746</v>
+        <v>0.09789509999999901</v>
       </c>
     </row>
     <row r="340" spans="1:4">
@@ -5265,10 +5265,10 @@
         <v>1101076.41</v>
       </c>
       <c r="C340" s="1">
-        <v>0.002897644774988217</v>
+        <v>0.002897644774987995</v>
       </c>
       <c r="D340" s="1">
-        <v>0.1010764099999977</v>
+        <v>0.101076409999999</v>
       </c>
     </row>
     <row r="341" spans="1:4">
@@ -5282,7 +5282,7 @@
         <v>0</v>
       </c>
       <c r="D341" s="1">
-        <v>0.1010764099999977</v>
+        <v>0.101076409999999</v>
       </c>
     </row>
     <row r="342" spans="1:4">
@@ -5296,7 +5296,7 @@
         <v>0</v>
       </c>
       <c r="D342" s="1">
-        <v>0.1010764099999977</v>
+        <v>0.101076409999999</v>
       </c>
     </row>
     <row r="343" spans="1:4">
@@ -5310,7 +5310,7 @@
         <v>0.01006707608966018</v>
       </c>
       <c r="D343" s="1">
-        <v>0.1121610299999976</v>
+        <v>0.1121610299999989</v>
       </c>
     </row>
     <row r="344" spans="1:4">
@@ -5321,10 +5321,10 @@
         <v>1113721.23</v>
       </c>
       <c r="C344" s="1">
-        <v>0.001402854404995768</v>
+        <v>0.001402854404995546</v>
       </c>
       <c r="D344" s="1">
-        <v>0.1137212299999977</v>
+        <v>0.1137212299999988</v>
       </c>
     </row>
     <row r="345" spans="1:4">
@@ -5338,7 +5338,7 @@
         <v>-0.007203535125212768</v>
       </c>
       <c r="D345" s="1">
-        <v>0.1056984999999975</v>
+        <v>0.1056984999999986</v>
       </c>
     </row>
     <row r="346" spans="1:4">
@@ -5352,7 +5352,7 @@
         <v>0.001937535413134794</v>
       </c>
       <c r="D346" s="1">
-        <v>0.1078408299999976</v>
+        <v>0.1078408299999987</v>
       </c>
     </row>
     <row r="347" spans="1:4">
@@ -5366,7 +5366,7 @@
         <v>0</v>
       </c>
       <c r="D347" s="1">
-        <v>0.1078408299999976</v>
+        <v>0.1078408299999987</v>
       </c>
     </row>
     <row r="348" spans="1:4">
@@ -5380,7 +5380,7 @@
         <v>0</v>
       </c>
       <c r="D348" s="1">
-        <v>0.1078408299999976</v>
+        <v>0.1078408299999987</v>
       </c>
     </row>
     <row r="349" spans="1:4">
@@ -5394,7 +5394,7 @@
         <v>0</v>
       </c>
       <c r="D349" s="1">
-        <v>0.1078408299999976</v>
+        <v>0.1078408299999987</v>
       </c>
     </row>
     <row r="350" spans="1:4">
@@ -5408,7 +5408,7 @@
         <v>-0.006011125262462169</v>
       </c>
       <c r="D350" s="1">
-        <v>0.1011814599999976</v>
+        <v>0.1011814599999987</v>
       </c>
     </row>
     <row r="351" spans="1:4">
@@ -5416,13 +5416,13 @@
         <v>38153</v>
       </c>
       <c r="B351">
-        <v>1104704.14</v>
+        <v>1104704.139999999</v>
       </c>
       <c r="C351" s="1">
-        <v>0.00319900046264876</v>
+        <v>0.003199000462648316</v>
       </c>
       <c r="D351" s="1">
-        <v>0.1047041399999979</v>
+        <v>0.1047041399999984</v>
       </c>
     </row>
     <row r="352" spans="1:4">
@@ -5430,13 +5430,13 @@
         <v>38154</v>
       </c>
       <c r="B352">
-        <v>1105653.39</v>
+        <v>1105653.389999999</v>
       </c>
       <c r="C352" s="1">
         <v>0.0008592798430175907</v>
       </c>
       <c r="D352" s="1">
-        <v>0.1056533899999981</v>
+        <v>0.1056533899999985</v>
       </c>
     </row>
     <row r="353" spans="1:4">
@@ -5444,13 +5444,13 @@
         <v>38155</v>
       </c>
       <c r="B353">
-        <v>1104575.26</v>
+        <v>1104575.259999999</v>
       </c>
       <c r="C353" s="1">
-        <v>-0.0009751066742533787</v>
+        <v>-0.0009751066742536008</v>
       </c>
       <c r="D353" s="1">
-        <v>0.1045752599999983</v>
+        <v>0.1045752599999985</v>
       </c>
     </row>
     <row r="354" spans="1:4">
@@ -5458,13 +5458,13 @@
         <v>38156</v>
       </c>
       <c r="B354">
-        <v>1105822.2</v>
+        <v>1105822.199999999</v>
       </c>
       <c r="C354" s="1">
-        <v>0.001128886410148189</v>
+        <v>0.001128886410148411</v>
       </c>
       <c r="D354" s="1">
-        <v>0.1058221999999982</v>
+        <v>0.1058221999999986</v>
       </c>
     </row>
     <row r="355" spans="1:4">
@@ -5472,13 +5472,13 @@
         <v>38157</v>
       </c>
       <c r="B355">
-        <v>1105822.2</v>
+        <v>1105822.199999999</v>
       </c>
       <c r="C355" s="1">
         <v>0</v>
       </c>
       <c r="D355" s="1">
-        <v>0.1058221999999982</v>
+        <v>0.1058221999999986</v>
       </c>
     </row>
     <row r="356" spans="1:4">
@@ -5486,13 +5486,13 @@
         <v>38158</v>
       </c>
       <c r="B356">
-        <v>1105822.2</v>
+        <v>1105822.199999999</v>
       </c>
       <c r="C356" s="1">
         <v>0</v>
       </c>
       <c r="D356" s="1">
-        <v>0.1058221999999982</v>
+        <v>0.1058221999999986</v>
       </c>
     </row>
     <row r="357" spans="1:4">
@@ -5500,13 +5500,13 @@
         <v>38159</v>
       </c>
       <c r="B357">
-        <v>1102571.18</v>
+        <v>1102571.179999999</v>
       </c>
       <c r="C357" s="1">
-        <v>-0.002939912040109016</v>
+        <v>-0.002939912040109127</v>
       </c>
       <c r="D357" s="1">
-        <v>0.1025711799999984</v>
+        <v>0.1025711799999987</v>
       </c>
     </row>
     <row r="358" spans="1:4">
@@ -5514,13 +5514,13 @@
         <v>38160</v>
       </c>
       <c r="B358">
-        <v>1103507.6</v>
+        <v>1103507.599999999</v>
       </c>
       <c r="C358" s="1">
-        <v>0.0008493057110379176</v>
+        <v>0.0008493057110381397</v>
       </c>
       <c r="D358" s="1">
-        <v>0.1035075999999981</v>
+        <v>0.1035075999999988</v>
       </c>
     </row>
   </sheetData>

</xml_diff>